<commit_message>
Added Updated time sheet - Chitrarasu
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25216"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B82235F-5AE0-49AB-99DB-FCA0A751A7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1024BF58-8922-47F8-8919-4F696072C976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="17" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="340">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1324,70 +1324,82 @@
     <t>Modified HTML layouts&lt;Educational details&gt;</t>
   </si>
   <si>
+    <t>Reviewed estimation sheet</t>
+  </si>
+  <si>
+    <t>Worked on HTML Layout for Wizard page</t>
+  </si>
+  <si>
+    <t>Reviewed HTML layout(Login,Forgot Password,Chnage Password,User Creation)</t>
+  </si>
+  <si>
+    <t>Lunch Break</t>
+  </si>
+  <si>
+    <t>Typescript topic</t>
+  </si>
+  <si>
+    <t>Working on HTML layout for wizard Layout</t>
+  </si>
+  <si>
+    <t>Worked on HTML layout for User Creation Page</t>
+  </si>
+  <si>
     <t>Team Meeting</t>
   </si>
   <si>
+    <t>Learned Angular &lt;Topics&gt;</t>
+  </si>
+  <si>
+    <t>Worked on HTML Layout for Wizard(skill)page</t>
+  </si>
+  <si>
+    <t>HTML layout wizard(In progress)</t>
+  </si>
+  <si>
+    <t>Harini</t>
+  </si>
+  <si>
+    <t>Worked on HTML layout for login page</t>
+  </si>
+  <si>
+    <t>Morning break</t>
+  </si>
+  <si>
+    <t>Reviewed the HTML layout</t>
+  </si>
+  <si>
+    <t>Customer meeting</t>
+  </si>
+  <si>
+    <t>Lunch break</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploration on typescript topics </t>
+  </si>
+  <si>
+    <t>Modified changes in Login page(HTML)</t>
+  </si>
+  <si>
+    <t>Worked on HTML layout for home page</t>
+  </si>
+  <si>
+    <t>worked on HTML layout for Change Password</t>
+  </si>
+  <si>
+    <t>worked on HTML layout for Forgot Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular session </t>
+  </si>
+  <si>
+    <t>Working on HTML layout for Change Password</t>
+  </si>
+  <si>
     <t>Soft Skill</t>
   </si>
   <si>
-    <t>Learned Angular &lt;Topics&gt;</t>
-  </si>
-  <si>
     <t>Working on HTML layout</t>
-  </si>
-  <si>
-    <t>Worked on HTML layout for User Creation Page</t>
-  </si>
-  <si>
-    <t>Lunch Break</t>
-  </si>
-  <si>
-    <t>Worked on HTML Layout for Wizard(skill)page</t>
-  </si>
-  <si>
-    <t>HTML layout wizard(In progress)</t>
-  </si>
-  <si>
-    <t>Harini</t>
-  </si>
-  <si>
-    <t>Reviewed estimation sheet</t>
-  </si>
-  <si>
-    <t>Worked on HTML layout for login page</t>
-  </si>
-  <si>
-    <t>Morning break</t>
-  </si>
-  <si>
-    <t>Reviewed the HTML layout</t>
-  </si>
-  <si>
-    <t>Customer meeting</t>
-  </si>
-  <si>
-    <t>Lunch break</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exploration on typescript topics </t>
-  </si>
-  <si>
-    <t>Modified changes in Login page(HTML)</t>
-  </si>
-  <si>
-    <t>Worked on HTML layout for home page</t>
-  </si>
-  <si>
-    <t>worked on HTML layout for Change Password</t>
-  </si>
-  <si>
-    <t>worked on HTML layout for Forgot Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angular session </t>
-  </si>
-  <si>
-    <t>Working on HTML layout for Change Password</t>
   </si>
   <si>
     <t>Worked on Web api(SOC,Factory pattern)</t>
@@ -5235,8 +5247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A84DE649-C5F3-4109-BE1F-71D1CBA3BD0C}">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5578,14 +5590,14 @@
         <v>290</v>
       </c>
       <c r="D17" s="108">
-        <v>0.41666666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="E17" s="108">
-        <v>0.4236111111111111</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="F17" s="108">
         <f t="shared" si="0"/>
-        <v>6.9444444444444198E-3</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H17" s="106" t="s">
         <v>291</v>
@@ -5600,95 +5612,95 @@
         <v>308</v>
       </c>
       <c r="C18" s="107" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D18" s="108">
-        <v>0.42708333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="E18" s="108">
-        <v>0.45833333333333331</v>
+        <v>0.4375</v>
       </c>
       <c r="F18" s="108">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>4.1666666666666685E-2</v>
       </c>
       <c r="H18" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I18" s="108">
         <f t="shared" ref="I18" si="8">SUMIFS(F17:F31, C17:C31,H18)</f>
-        <v>0.22916666666666674</v>
+        <v>0.27083333333333331</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="121"/>
       <c r="B19" s="107" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C19" s="107" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D19" s="108">
+        <v>0.4375</v>
+      </c>
+      <c r="E19" s="108">
         <v>0.45833333333333331</v>
-      </c>
-      <c r="E19" s="108">
-        <v>0.47222222222222227</v>
       </c>
       <c r="F19" s="108">
         <f t="shared" si="0"/>
-        <v>1.3888888888888951E-2</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H19" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I19" s="108">
         <f t="shared" ref="I19" si="9">SUMIFS(F17:F31, C17:C31,H19)</f>
-        <v>7.2916666666666685E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="121"/>
       <c r="B20" s="107" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C20" s="107" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D20" s="108">
-        <v>0.47916666666666669</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E20" s="108">
         <v>0.52083333333333337</v>
       </c>
       <c r="F20" s="108">
         <f t="shared" si="0"/>
-        <v>4.1666666666666685E-2</v>
+        <v>6.2500000000000056E-2</v>
       </c>
       <c r="H20" s="109" t="s">
         <v>297</v>
       </c>
       <c r="I20" s="108">
         <f t="shared" ref="I20" si="10">SUMIFS(F17:F31, C17:C31,H20)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="121"/>
       <c r="B21" s="107" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C21" s="107" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D21" s="108">
-        <v>0.52083333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="E21" s="108">
-        <v>0.54166666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="F21" s="108">
         <f t="shared" si="0"/>
-        <v>2.0833333333333259E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H21" s="109" t="s">
         <v>300</v>
@@ -5701,20 +5713,20 @@
     <row r="22" spans="1:9">
       <c r="A22" s="121"/>
       <c r="B22" s="107" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>299</v>
       </c>
       <c r="D22" s="108">
-        <v>0.47222222222222227</v>
+        <v>0.57291666666666663</v>
       </c>
       <c r="E22" s="108">
-        <v>0.47916666666666669</v>
+        <v>0.59375</v>
       </c>
       <c r="F22" s="108">
         <f t="shared" si="0"/>
-        <v>6.9444444444444198E-3</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H22" s="109" t="s">
         <v>302</v>
@@ -5727,72 +5739,72 @@
     <row r="23" spans="1:9">
       <c r="A23" s="121"/>
       <c r="B23" s="107" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C23" s="107" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D23" s="108">
-        <v>0.65625</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="E23" s="108">
-        <v>0.66666666666666663</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="F23" s="108">
         <f t="shared" si="0"/>
-        <v>1.041666666666663E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H23" s="109" t="s">
         <v>299</v>
       </c>
       <c r="I23" s="108">
         <f t="shared" ref="I23" si="13">SUMIFS(F17:F31, C17:C31,H23)</f>
-        <v>3.8194444444444309E-2</v>
+        <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="121"/>
       <c r="B24" s="107" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C24" s="107" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D24" s="108">
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="E24" s="108">
-        <v>0.75</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="F24" s="108">
         <f t="shared" si="0"/>
-        <v>8.333333333333337E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H24" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I24" s="106">
         <f t="shared" ref="I24" si="14">SUM(I18:I23)</f>
-        <v>0.34027777777777773</v>
+        <v>0.375</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="121"/>
       <c r="B25" s="107" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C25" s="107" t="s">
         <v>290</v>
       </c>
       <c r="D25" s="108">
-        <v>0.75</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="E25" s="108">
-        <v>0.875</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="F25" s="108">
         <f t="shared" si="0"/>
-        <v>0.125</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="I25" s="110"/>
     </row>
@@ -5893,7 +5905,7 @@
     <row r="33" spans="1:9">
       <c r="A33" s="121"/>
       <c r="B33" s="107" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C33" s="107" t="s">
         <v>290</v>
@@ -5945,7 +5957,7 @@
     <row r="35" spans="1:9">
       <c r="A35" s="121"/>
       <c r="B35" s="107" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C35" s="107" t="s">
         <v>290</v>
@@ -5997,7 +6009,7 @@
     <row r="37" spans="1:9">
       <c r="A37" s="121"/>
       <c r="B37" s="107" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C37" s="107" t="s">
         <v>299</v>
@@ -6023,7 +6035,7 @@
     <row r="38" spans="1:9">
       <c r="A38" s="121"/>
       <c r="B38" s="107" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C38" s="107" t="s">
         <v>295</v>
@@ -6049,7 +6061,7 @@
     <row r="39" spans="1:9">
       <c r="A39" s="121"/>
       <c r="B39" s="107" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C39" s="107" t="s">
         <v>297</v>
@@ -6095,7 +6107,7 @@
     <row r="41" spans="1:9">
       <c r="A41" s="121"/>
       <c r="B41" s="107" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="C41" s="107" t="s">
         <v>290</v>
@@ -6126,7 +6138,7 @@
     <row r="43" spans="1:9">
       <c r="A43" s="121"/>
       <c r="B43" s="107" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="C43" s="107"/>
       <c r="D43" s="108"/>
@@ -6171,10 +6183,10 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="121" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="B47" s="107" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C47" s="107" t="s">
         <v>290</v>
@@ -6199,7 +6211,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="121"/>
       <c r="B48" s="107" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>290</v>
@@ -6225,7 +6237,7 @@
     <row r="49" spans="1:9">
       <c r="A49" s="121"/>
       <c r="B49" s="107" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C49" s="107" t="s">
         <v>299</v>
@@ -6251,7 +6263,7 @@
     <row r="50" spans="1:9">
       <c r="A50" s="121"/>
       <c r="B50" s="107" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C50" s="107" t="s">
         <v>290</v>
@@ -6277,7 +6289,7 @@
     <row r="51" spans="1:9">
       <c r="A51" s="121"/>
       <c r="B51" s="107" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C51" s="107" t="s">
         <v>290</v>
@@ -6303,7 +6315,7 @@
     <row r="52" spans="1:9">
       <c r="A52" s="121"/>
       <c r="B52" s="107" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C52" s="107" t="s">
         <v>299</v>
@@ -6355,7 +6367,7 @@
     <row r="54" spans="1:9">
       <c r="A54" s="121"/>
       <c r="B54" s="107" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C54" s="107" t="s">
         <v>297</v>
@@ -6381,7 +6393,7 @@
     <row r="55" spans="1:9">
       <c r="A55" s="121"/>
       <c r="B55" s="107" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C55" s="107" t="s">
         <v>290</v>
@@ -6401,7 +6413,7 @@
     <row r="56" spans="1:9">
       <c r="A56" s="121"/>
       <c r="B56" s="107" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C56" s="107" t="s">
         <v>290</v>
@@ -6478,7 +6490,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="107" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C62" s="107" t="s">
         <v>290</v>
@@ -6503,7 +6515,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="121"/>
       <c r="B63" s="107" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C63" s="107" t="s">
         <v>290</v>
@@ -6555,7 +6567,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="121"/>
       <c r="B65" s="107" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>290</v>
@@ -6607,7 +6619,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="121"/>
       <c r="B67" s="107" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>299</v>
@@ -6659,7 +6671,7 @@
     <row r="69" spans="1:9">
       <c r="A69" s="121"/>
       <c r="B69" s="107" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C69" s="107" t="s">
         <v>290</v>
@@ -6685,7 +6697,7 @@
     <row r="70" spans="1:9">
       <c r="A70" s="121"/>
       <c r="B70" s="107" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C70" s="107" t="s">
         <v>290</v>
@@ -6774,7 +6786,7 @@
         <v>67</v>
       </c>
       <c r="B77" s="107" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C77" s="107" t="s">
         <v>290</v>
@@ -6799,7 +6811,7 @@
     <row r="78" spans="1:9">
       <c r="A78" s="121"/>
       <c r="B78" s="107" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C78" s="107" t="s">
         <v>295</v>
@@ -6851,7 +6863,7 @@
     <row r="80" spans="1:9">
       <c r="A80" s="121"/>
       <c r="B80" s="107" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C80" s="107" t="s">
         <v>295</v>
@@ -6955,7 +6967,7 @@
     <row r="84" spans="1:9">
       <c r="A84" s="121"/>
       <c r="B84" s="107" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C84" s="107" t="s">
         <v>290</v>
@@ -6981,7 +6993,7 @@
     <row r="85" spans="1:9">
       <c r="A85" s="121"/>
       <c r="B85" s="107" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C85" s="107" t="s">
         <v>290</v>
@@ -7070,7 +7082,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="107" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C92" s="107" t="s">
         <v>290</v>
@@ -7095,7 +7107,7 @@
     <row r="93" spans="1:9">
       <c r="A93" s="121"/>
       <c r="B93" s="107" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="C93" s="107" t="s">
         <v>290</v>
@@ -7147,7 +7159,7 @@
     <row r="95" spans="1:9">
       <c r="A95" s="121"/>
       <c r="B95" s="107" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C95" s="107" t="s">
         <v>290</v>
@@ -7199,7 +7211,7 @@
     <row r="97" spans="1:9">
       <c r="A97" s="121"/>
       <c r="B97" s="107" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C97" s="107" t="s">
         <v>299</v>
@@ -7225,7 +7237,7 @@
     <row r="98" spans="1:9">
       <c r="A98" s="121"/>
       <c r="B98" s="107" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C98" s="107" t="s">
         <v>297</v>
@@ -7251,7 +7263,7 @@
     <row r="99" spans="1:9">
       <c r="A99" s="121"/>
       <c r="B99" s="107" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C99" s="107" t="s">
         <v>295</v>
@@ -7277,7 +7289,7 @@
     <row r="100" spans="1:9">
       <c r="A100" s="121"/>
       <c r="B100" s="107" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C100" s="107" t="s">
         <v>297</v>
@@ -7317,7 +7329,7 @@
     <row r="102" spans="1:9">
       <c r="A102" s="121"/>
       <c r="B102" s="107" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C102" s="107" t="s">
         <v>290</v>
@@ -7336,7 +7348,7 @@
     <row r="103" spans="1:9">
       <c r="A103" s="121"/>
       <c r="B103" s="107" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C103" s="107" t="s">
         <v>297</v>
@@ -7390,7 +7402,7 @@
         <v>19</v>
       </c>
       <c r="B107" s="115" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C107" s="107" t="s">
         <v>290</v>
@@ -7415,7 +7427,7 @@
     <row r="108" spans="1:9">
       <c r="A108" s="123"/>
       <c r="B108" s="115" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C108" s="107" t="s">
         <v>295</v>
@@ -7467,7 +7479,7 @@
     <row r="110" spans="1:9">
       <c r="A110" s="123"/>
       <c r="B110" s="115" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C110" s="107" t="s">
         <v>295</v>
@@ -7571,7 +7583,7 @@
     <row r="114" spans="1:9">
       <c r="A114" s="123"/>
       <c r="B114" s="115" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C114" s="107" t="s">
         <v>290</v>
@@ -7597,7 +7609,7 @@
     <row r="115" spans="1:9">
       <c r="A115" s="123"/>
       <c r="B115" s="115" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C115" s="107" t="s">
         <v>290</v>
@@ -7683,10 +7695,10 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" s="123" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="B122" s="115" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>290</v>
@@ -7711,7 +7723,7 @@
     <row r="123" spans="1:9">
       <c r="A123" s="123"/>
       <c r="B123" s="115" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C123" s="107" t="s">
         <v>295</v>
@@ -7763,7 +7775,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="123"/>
       <c r="B125" s="115" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>295</v>
@@ -7867,7 +7879,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="123"/>
       <c r="B129" s="115" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C129" s="107" t="s">
         <v>290</v>
@@ -7893,7 +7905,7 @@
     <row r="130" spans="1:9">
       <c r="A130" s="123"/>
       <c r="B130" s="115" t="s">
-        <v>310</v>
+        <v>332</v>
       </c>
       <c r="C130" s="107" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
commited time sheet by kishore
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C71CDFAC-18BA-4903-AFAA-BF67BB613039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C79A58A1-DF0E-4014-9906-AAF6CB61F06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="20" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2994" uniqueCount="491">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1621,6 +1621,9 @@
     <t>Exploration on angular topics</t>
   </si>
   <si>
+    <t>Entering Timesheet</t>
+  </si>
+  <si>
     <t>Explored on Angular(components)</t>
   </si>
   <si>
@@ -1630,6 +1633,9 @@
     <t>Worked on Angular(components)</t>
   </si>
   <si>
+    <t xml:space="preserve">College project </t>
+  </si>
+  <si>
     <t>Modified on HTML (achivements)</t>
   </si>
   <si>
@@ -1640,6 +1646,12 @@
   </si>
   <si>
     <t>Worked on Angular topics</t>
+  </si>
+  <si>
+    <t>Modifications on HTML layout Page(Home page)</t>
+  </si>
+  <si>
+    <t>Explored on Web Api</t>
   </si>
   <si>
     <t>Explored Web API, Angular</t>
@@ -16561,8 +16573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30934AA5-FE34-4D93-9147-E487E171875A}">
   <dimension ref="A1:Q142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="P63" sqref="P63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17196,20 +17208,20 @@
         <v>54</v>
       </c>
       <c r="B31" s="107" t="s">
-        <v>356</v>
+        <v>404</v>
       </c>
       <c r="C31" s="107" t="s">
         <v>290</v>
       </c>
       <c r="D31" s="108">
-        <v>0.35416666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="E31" s="108">
-        <v>0.39583333333333331</v>
+        <v>0.38541666666666669</v>
       </c>
       <c r="F31" s="108">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>1.0416666666666685E-2</v>
       </c>
       <c r="H31" s="106" t="s">
         <v>291</v>
@@ -17221,10 +17233,10 @@
     <row r="32" spans="1:9">
       <c r="A32" s="132"/>
       <c r="B32" s="107" t="s">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="C32" s="107" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D32" s="108">
         <v>0.39583333333333331</v>
@@ -17241,7 +17253,7 @@
       </c>
       <c r="I32" s="108">
         <f t="shared" ref="I32" si="2">SUMIFS(F31:F45, C31:C45,H32)</f>
-        <v>0.28125000000000011</v>
+        <v>0.25000000000000017</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -17256,18 +17268,18 @@
         <v>0.4375</v>
       </c>
       <c r="E33" s="108">
-        <v>0.44444444444444442</v>
+        <v>0.46875</v>
       </c>
       <c r="F33" s="108">
         <f t="shared" si="0"/>
-        <v>6.9444444444444198E-3</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H33" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I33" s="108">
         <f t="shared" ref="I33" si="3">SUMIFS(F31:F45, C31:C45,H33)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -17293,7 +17305,7 @@
       </c>
       <c r="I34" s="108">
         <f t="shared" ref="I34" si="4">SUMIFS(F31:F45, C31:C45,H34)</f>
-        <v>6.25E-2</v>
+        <v>0.10416666666666669</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -17371,7 +17383,7 @@
       </c>
       <c r="I37" s="108">
         <f t="shared" ref="I37" si="7">SUMIFS(F31:F45, C31:C45,H37)</f>
-        <v>4.8611111111111049E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -17397,7 +17409,7 @@
       </c>
       <c r="I38" s="106">
         <f t="shared" ref="I38" si="8">SUM(I32:I37)</f>
-        <v>0.49305555555555564</v>
+        <v>0.48611111111111127</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -17516,7 +17528,7 @@
         <v>318</v>
       </c>
       <c r="B46" s="107" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C46" s="107" t="s">
         <v>297</v>
@@ -17541,7 +17553,7 @@
     <row r="47" spans="1:9">
       <c r="A47" s="132"/>
       <c r="B47" s="107" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C47" s="107" t="s">
         <v>290</v>
@@ -17567,7 +17579,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="132"/>
       <c r="B48" s="107" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>290</v>
@@ -17587,7 +17599,7 @@
       </c>
       <c r="I48" s="108">
         <f>SUMIFS(F46:F59, C46:C59,H48)</f>
-        <v>0</v>
+        <v>0.14583333333333326</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -17618,13 +17630,21 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="132"/>
-      <c r="B50" s="107"/>
-      <c r="C50" s="107"/>
-      <c r="D50" s="108"/>
-      <c r="E50" s="108"/>
+      <c r="B50" s="107" t="s">
+        <v>408</v>
+      </c>
+      <c r="C50" s="107" t="s">
+        <v>295</v>
+      </c>
+      <c r="D50" s="108">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E50" s="108">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F50" s="108">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.14583333333333326</v>
       </c>
       <c r="H50" s="109" t="s">
         <v>300</v>
@@ -17685,7 +17705,7 @@
       </c>
       <c r="I53" s="106">
         <f t="shared" ref="I53" si="9">SUM(I47:I52)</f>
-        <v>0.17708333333333326</v>
+        <v>0.32291666666666652</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -17761,7 +17781,7 @@
         <v>62</v>
       </c>
       <c r="B60" s="107" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="C60" s="107" t="s">
         <v>290</v>
@@ -17786,7 +17806,7 @@
     <row r="61" spans="1:9">
       <c r="A61" s="132"/>
       <c r="B61" s="107" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C61" s="107" t="s">
         <v>297</v>
@@ -17806,13 +17826,13 @@
       </c>
       <c r="I61" s="108">
         <f t="shared" ref="I61" si="10">SUMIFS(F60:F74, C60:C74,H61)</f>
-        <v>0.17361111111111116</v>
+        <v>0.21527777777777779</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="132"/>
       <c r="B62" s="107" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="C62" s="107" t="s">
         <v>290</v>
@@ -17858,7 +17878,7 @@
       </c>
       <c r="I63" s="108">
         <f t="shared" ref="I63" si="12">SUMIFS(F60:F74, C60:C74,H63)</f>
-        <v>4.8611111111111105E-2</v>
+        <v>9.0277777777777846E-2</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -17890,7 +17910,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="132"/>
       <c r="B65" s="107" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>290</v>
@@ -17915,13 +17935,21 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="132"/>
-      <c r="B66" s="107"/>
-      <c r="C66" s="107"/>
-      <c r="D66" s="108"/>
-      <c r="E66" s="108"/>
+      <c r="B66" s="107" t="s">
+        <v>413</v>
+      </c>
+      <c r="C66" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D66" s="108">
+        <v>0.6875</v>
+      </c>
+      <c r="E66" s="108">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F66" s="108">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H66" s="109" t="s">
         <v>299</v>
@@ -17933,20 +17961,28 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="132"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="107"/>
-      <c r="D67" s="108"/>
-      <c r="E67" s="108"/>
+      <c r="B67" s="107" t="s">
+        <v>414</v>
+      </c>
+      <c r="C67" s="107" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" s="108">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E67" s="108">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="F67" s="108">
         <f t="shared" ref="F67:F130" si="16">E67-D67</f>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="H67" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I67" s="106">
         <f t="shared" ref="I67" si="17">SUM(I61:I66)</f>
-        <v>0.2638888888888889</v>
+        <v>0.34722222222222227</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -18953,7 +18989,7 @@
         <v>339</v>
       </c>
       <c r="B120" s="115" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="C120" s="107" t="s">
         <v>297</v>
@@ -19004,7 +19040,7 @@
     <row r="122" spans="1:9">
       <c r="A122" s="136"/>
       <c r="B122" s="115" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>300</v>
@@ -19030,7 +19066,7 @@
     <row r="123" spans="1:9">
       <c r="A123" s="136"/>
       <c r="B123" s="115" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C123" s="107" t="s">
         <v>290</v>
@@ -19082,7 +19118,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="136"/>
       <c r="B125" s="115" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>290</v>
@@ -19375,7 +19411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F5FAB4-9E65-460D-998C-A6B05E121251}">
   <dimension ref="A1:Q142"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
@@ -19419,7 +19455,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="107" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="C2" s="107" t="s">
         <v>290</v>
@@ -19505,7 +19541,7 @@
     <row r="5" spans="1:17">
       <c r="A5" s="132"/>
       <c r="B5" s="107" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C5" s="107" t="s">
         <v>290</v>
@@ -19534,7 +19570,7 @@
     <row r="6" spans="1:17">
       <c r="A6" s="132"/>
       <c r="B6" s="107" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>290</v>
@@ -19563,7 +19599,7 @@
     <row r="7" spans="1:17">
       <c r="A7" s="132"/>
       <c r="B7" s="107" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C7" s="107" t="s">
         <v>297</v>
@@ -20330,7 +20366,7 @@
         <v>318</v>
       </c>
       <c r="B46" s="107" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C46" s="107" t="s">
         <v>297</v>
@@ -20355,7 +20391,7 @@
     <row r="47" spans="1:9">
       <c r="A47" s="132"/>
       <c r="B47" s="107" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C47" s="107" t="s">
         <v>290</v>
@@ -20381,7 +20417,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="132"/>
       <c r="B48" s="107" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>300</v>
@@ -20407,7 +20443,7 @@
     <row r="49" spans="1:9">
       <c r="A49" s="132"/>
       <c r="B49" s="107" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C49" s="107" t="s">
         <v>290</v>
@@ -20433,7 +20469,7 @@
     <row r="50" spans="1:9">
       <c r="A50" s="132"/>
       <c r="B50" s="107" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="C50" s="107" t="s">
         <v>290</v>
@@ -20583,7 +20619,7 @@
         <v>62</v>
       </c>
       <c r="B60" s="107" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="C60" s="107" t="s">
         <v>290</v>
@@ -20608,7 +20644,7 @@
     <row r="61" spans="1:9">
       <c r="A61" s="132"/>
       <c r="B61" s="107" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="C61" s="107" t="s">
         <v>290</v>
@@ -20634,7 +20670,7 @@
     <row r="62" spans="1:9">
       <c r="A62" s="132"/>
       <c r="B62" s="107" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="C62" s="107" t="s">
         <v>300</v>
@@ -20660,7 +20696,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="132"/>
       <c r="B63" s="107" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C63" s="107" t="s">
         <v>290</v>
@@ -20686,7 +20722,7 @@
     <row r="64" spans="1:9">
       <c r="A64" s="132"/>
       <c r="B64" s="107" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C64" s="107" t="s">
         <v>297</v>
@@ -20712,7 +20748,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="132"/>
       <c r="B65" s="107" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>290</v>
@@ -21744,7 +21780,7 @@
         <v>339</v>
       </c>
       <c r="B120" s="115" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="C120" s="107" t="s">
         <v>297</v>
@@ -21795,7 +21831,7 @@
     <row r="122" spans="1:9">
       <c r="A122" s="136"/>
       <c r="B122" s="115" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>300</v>
@@ -21821,7 +21857,7 @@
     <row r="123" spans="1:9">
       <c r="A123" s="136"/>
       <c r="B123" s="115" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C123" s="107" t="s">
         <v>290</v>
@@ -21873,7 +21909,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="136"/>
       <c r="B125" s="115" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>290</v>
@@ -22166,7 +22202,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEFA632-027C-44B7-B2E8-75A517756B1E}">
   <dimension ref="A1:Q142"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
@@ -22210,7 +22246,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="107" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="C2" s="107" t="s">
         <v>290</v>
@@ -22267,7 +22303,7 @@
     <row r="4" spans="1:17">
       <c r="A4" s="132"/>
       <c r="B4" s="107" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="C4" s="107" t="s">
         <v>290</v>
@@ -22296,7 +22332,7 @@
     <row r="5" spans="1:17">
       <c r="A5" s="132"/>
       <c r="B5" s="107" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="C5" s="107" t="s">
         <v>290</v>
@@ -22354,7 +22390,7 @@
     <row r="7" spans="1:17">
       <c r="A7" s="132"/>
       <c r="B7" s="107" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="C7" s="107" t="s">
         <v>290</v>
@@ -22409,7 +22445,7 @@
     <row r="9" spans="1:17">
       <c r="A9" s="132"/>
       <c r="B9" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C9" s="107" t="s">
         <v>297</v>
@@ -22455,7 +22491,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="132"/>
       <c r="B11" s="107" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="C11" s="107" t="s">
         <v>290</v>
@@ -22833,7 +22869,7 @@
         <v>54</v>
       </c>
       <c r="B31" s="107" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C31" s="107" t="s">
         <v>290</v>
@@ -23153,7 +23189,7 @@
         <v>318</v>
       </c>
       <c r="B46" s="107" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="C46" s="107" t="s">
         <v>290</v>
@@ -23204,7 +23240,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="132"/>
       <c r="B48" s="107" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>290</v>
@@ -23256,7 +23292,7 @@
     <row r="50" spans="1:9">
       <c r="A50" s="132"/>
       <c r="B50" s="107" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C50" s="107" t="s">
         <v>290</v>
@@ -23308,7 +23344,7 @@
     <row r="52" spans="1:9">
       <c r="A52" s="132"/>
       <c r="B52" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C52" s="107" t="s">
         <v>297</v>
@@ -23430,7 +23466,7 @@
         <v>62</v>
       </c>
       <c r="B60" s="107" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C60" s="107" t="s">
         <v>290</v>
@@ -23455,7 +23491,7 @@
     <row r="61" spans="1:9">
       <c r="A61" s="132"/>
       <c r="B61" s="107" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="C61" s="107" t="s">
         <v>290</v>
@@ -23507,7 +23543,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="132"/>
       <c r="B63" s="107" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="C63" s="107" t="s">
         <v>290</v>
@@ -23559,7 +23595,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="132"/>
       <c r="B65" s="107" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>290</v>
@@ -23611,7 +23647,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="132"/>
       <c r="B67" s="107" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>297</v>
@@ -23726,7 +23762,7 @@
         <v>67</v>
       </c>
       <c r="B75" s="107" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="C75" s="107" t="s">
         <v>297</v>
@@ -23751,7 +23787,7 @@
     <row r="76" spans="1:9">
       <c r="A76" s="132"/>
       <c r="B76" s="107" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C76" s="107" t="s">
         <v>290</v>
@@ -23803,7 +23839,7 @@
     <row r="78" spans="1:9">
       <c r="A78" s="132"/>
       <c r="B78" s="107" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="C78" s="107" t="s">
         <v>290</v>
@@ -23829,7 +23865,7 @@
     <row r="79" spans="1:9">
       <c r="A79" s="132"/>
       <c r="B79" s="107" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C79" s="107" t="s">
         <v>299</v>
@@ -23881,7 +23917,7 @@
     <row r="81" spans="1:9">
       <c r="A81" s="132"/>
       <c r="B81" s="107" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="C81" s="107" t="s">
         <v>290</v>
@@ -23907,7 +23943,7 @@
     <row r="82" spans="1:9">
       <c r="A82" s="132"/>
       <c r="B82" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="C82" s="107" t="s">
         <v>297</v>
@@ -23933,7 +23969,7 @@
     <row r="83" spans="1:9">
       <c r="A83" s="132"/>
       <c r="B83" s="107" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="C83" s="107" t="s">
         <v>290</v>
@@ -23953,7 +23989,7 @@
     <row r="84" spans="1:9">
       <c r="A84" s="132"/>
       <c r="B84" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C84" s="107" t="s">
         <v>297</v>
@@ -24629,7 +24665,7 @@
         <v>339</v>
       </c>
       <c r="B120" s="115" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C120" s="107" t="s">
         <v>290</v>
@@ -24654,7 +24690,7 @@
     <row r="121" spans="1:9">
       <c r="A121" s="136"/>
       <c r="B121" s="115" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C121" s="107" t="s">
         <v>290</v>
@@ -24706,7 +24742,7 @@
     <row r="123" spans="1:9">
       <c r="A123" s="136"/>
       <c r="B123" s="107" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="C123" s="107" t="s">
         <v>290</v>
@@ -24758,7 +24794,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="136"/>
       <c r="B125" s="107" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>290</v>
@@ -24810,7 +24846,7 @@
     <row r="127" spans="1:9">
       <c r="A127" s="136"/>
       <c r="B127" s="107" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="C127" s="107" t="s">
         <v>295</v>
@@ -24856,7 +24892,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="136"/>
       <c r="B129" s="115" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="C129" s="107" t="s">
         <v>297</v>
@@ -25131,7 +25167,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="107" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C2" s="107" t="s">
         <v>290</v>
@@ -25159,7 +25195,7 @@
     <row r="3" spans="1:17">
       <c r="A3" s="132"/>
       <c r="B3" s="107" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="C3" s="107" t="s">
         <v>290</v>
@@ -25217,7 +25253,7 @@
     <row r="5" spans="1:17">
       <c r="A5" s="132"/>
       <c r="B5" s="107" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="C5" s="107" t="s">
         <v>290</v>
@@ -25246,7 +25282,7 @@
     <row r="6" spans="1:17">
       <c r="A6" s="132"/>
       <c r="B6" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>297</v>
@@ -25275,7 +25311,7 @@
     <row r="7" spans="1:17">
       <c r="A7" s="132"/>
       <c r="B7" s="107" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="C7" s="107" t="s">
         <v>299</v>
@@ -25330,7 +25366,7 @@
     <row r="9" spans="1:17">
       <c r="A9" s="132"/>
       <c r="B9" s="107" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="C9" s="107" t="s">
         <v>290</v>
@@ -25376,7 +25412,7 @@
     <row r="11" spans="1:17">
       <c r="A11" s="132"/>
       <c r="B11" s="107" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C11" s="107" t="s">
         <v>290</v>
@@ -25396,7 +25432,7 @@
     <row r="12" spans="1:17">
       <c r="A12" s="132"/>
       <c r="B12" s="107" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="C12" s="107" t="s">
         <v>290</v>
@@ -25461,7 +25497,7 @@
         <v>48</v>
       </c>
       <c r="B17" s="107" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="C17" s="107" t="s">
         <v>290</v>
@@ -25512,7 +25548,7 @@
     <row r="19" spans="1:9">
       <c r="A19" s="132"/>
       <c r="B19" s="107" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="C19" s="107" t="s">
         <v>290</v>
@@ -25538,7 +25574,7 @@
     <row r="20" spans="1:9">
       <c r="A20" s="132"/>
       <c r="B20" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C20" s="107" t="s">
         <v>297</v>
@@ -25564,7 +25600,7 @@
     <row r="21" spans="1:9">
       <c r="A21" s="132"/>
       <c r="B21" s="107" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C21" s="107" t="s">
         <v>299</v>
@@ -25590,7 +25626,7 @@
     <row r="22" spans="1:9">
       <c r="A22" s="132"/>
       <c r="B22" s="107" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>290</v>
@@ -25668,7 +25704,7 @@
     <row r="25" spans="1:9">
       <c r="A25" s="132"/>
       <c r="B25" s="107" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C25" s="107" t="s">
         <v>290</v>
@@ -25723,7 +25759,7 @@
         <v>54</v>
       </c>
       <c r="B29" s="107" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="C29" s="107" t="s">
         <v>290</v>
@@ -26043,7 +26079,7 @@
         <v>318</v>
       </c>
       <c r="B44" s="107" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="C44" s="107" t="s">
         <v>290</v>
@@ -26094,7 +26130,7 @@
     <row r="46" spans="1:9">
       <c r="A46" s="132"/>
       <c r="B46" s="107" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="C46" s="107" t="s">
         <v>290</v>
@@ -26120,7 +26156,7 @@
     <row r="47" spans="1:9">
       <c r="A47" s="132"/>
       <c r="B47" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C47" s="107" t="s">
         <v>297</v>
@@ -26146,7 +26182,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="132"/>
       <c r="B48" s="107" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>299</v>
@@ -26198,7 +26234,7 @@
     <row r="50" spans="1:9">
       <c r="A50" s="132"/>
       <c r="B50" s="107" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="C50" s="107" t="s">
         <v>290</v>
@@ -26250,7 +26286,7 @@
     <row r="52" spans="1:9">
       <c r="A52" s="132"/>
       <c r="B52" s="107" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="C52" s="107" t="s">
         <v>290</v>
@@ -26270,7 +26306,7 @@
     <row r="53" spans="1:9">
       <c r="A53" s="132"/>
       <c r="B53" s="107" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="C53" s="107" t="s">
         <v>290</v>
@@ -26336,7 +26372,7 @@
         <v>62</v>
       </c>
       <c r="B58" s="107" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="C58" s="107" t="s">
         <v>297</v>
@@ -26413,7 +26449,7 @@
     <row r="61" spans="1:9">
       <c r="A61" s="132"/>
       <c r="B61" s="107" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C61" s="107" t="s">
         <v>295</v>
@@ -26465,7 +26501,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="132"/>
       <c r="B63" s="107" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="C63" s="107" t="s">
         <v>295</v>
@@ -26517,7 +26553,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="132"/>
       <c r="B65" s="107" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>295</v>
@@ -26564,7 +26600,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="132"/>
       <c r="B67" s="107" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>290</v>
@@ -26584,7 +26620,7 @@
     <row r="68" spans="1:9">
       <c r="A68" s="132"/>
       <c r="B68" s="107" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C68" s="107" t="s">
         <v>290</v>
@@ -26661,7 +26697,7 @@
         <v>67</v>
       </c>
       <c r="B74" s="107" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C74" s="107" t="s">
         <v>290</v>
@@ -26712,7 +26748,7 @@
     <row r="76" spans="1:9">
       <c r="A76" s="132"/>
       <c r="B76" s="107" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="C76" s="107" t="s">
         <v>290</v>
@@ -26738,7 +26774,7 @@
     <row r="77" spans="1:9">
       <c r="A77" s="132"/>
       <c r="B77" s="107" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="C77" s="107" t="s">
         <v>297</v>
@@ -27581,7 +27617,7 @@
         <v>339</v>
       </c>
       <c r="B119" s="115" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="C119" s="107" t="s">
         <v>290</v>
@@ -27606,7 +27642,7 @@
     <row r="120" spans="1:9">
       <c r="A120" s="136"/>
       <c r="B120" s="115" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="C120" s="107" t="s">
         <v>297</v>
@@ -27658,7 +27694,7 @@
     <row r="122" spans="1:9">
       <c r="A122" s="136"/>
       <c r="B122" s="107" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>290</v>
@@ -27684,7 +27720,7 @@
     <row r="123" spans="1:9">
       <c r="A123" s="136"/>
       <c r="B123" s="107" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="C123" s="107" t="s">
         <v>295</v>
@@ -27736,7 +27772,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="136"/>
       <c r="B125" s="107" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>290</v>
@@ -27788,7 +27824,7 @@
     <row r="127" spans="1:9">
       <c r="A127" s="136"/>
       <c r="B127" s="107" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
       <c r="C127" s="107" t="s">
         <v>290</v>
@@ -27828,7 +27864,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="136"/>
       <c r="B129" s="115" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="C129" s="107" t="s">
         <v>290</v>

</xml_diff>

<commit_message>
Timesheet updated by Nagaraj
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56161D04-CFAE-4EB8-B5A1-0F4A70E3A2FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9905E4B-236A-4894-9A6D-D9A5AFE36B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="24" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3172" uniqueCount="530">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1992,9 +1992,6 @@
   </si>
   <si>
     <t>Worked on angular and web api integration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implemented </t>
   </si>
   <si>
     <t>Explored on Data Binding</t>
@@ -2163,7 +2160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -2556,11 +2553,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2914,6 +2935,11 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -25216,7 +25242,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9EFCF2-B647-4263-9741-7AEEC9FEC381}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="R15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -28151,8 +28177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448AE304-61C3-4727-BB61-AC5EFF7EF149}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29778,7 +29804,7 @@
       </c>
       <c r="I75" s="108">
         <f>SUMIFS(F74:F86, C74:C86,H75)</f>
-        <v>0.15625000000000006</v>
+        <v>0.20833333333333331</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -29934,12 +29960,12 @@
       </c>
       <c r="I81" s="106">
         <f t="shared" ref="I81" si="15">SUM(I75:I80)</f>
-        <v>0.35069444444444442</v>
+        <v>0.40277777777777768</v>
       </c>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="132"/>
-      <c r="B82" s="107" t="s">
+      <c r="B82" s="111" t="s">
         <v>452</v>
       </c>
       <c r="C82" s="107" t="s">
@@ -29958,11 +29984,11 @@
       <c r="I82" s="110"/>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="132"/>
-      <c r="B83" s="107" t="s">
+      <c r="A83" s="137"/>
+      <c r="B83" s="113" t="s">
         <v>524</v>
       </c>
-      <c r="C83" s="107" t="s">
+      <c r="C83" s="115" t="s">
         <v>290</v>
       </c>
       <c r="D83" s="108">
@@ -29978,11 +30004,11 @@
       <c r="I83" s="110"/>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="132"/>
-      <c r="B84" s="107" t="s">
+      <c r="A84" s="137"/>
+      <c r="B84" s="113" t="s">
         <v>525</v>
       </c>
-      <c r="C84" s="111" t="s">
+      <c r="C84" s="116" t="s">
         <v>297</v>
       </c>
       <c r="D84" s="112">
@@ -29997,36 +30023,45 @@
       </c>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="132"/>
-      <c r="C85" s="113"/>
-      <c r="D85" s="114"/>
-      <c r="E85" s="114"/>
-      <c r="F85" s="114"/>
+      <c r="A85" s="137"/>
+      <c r="B85" s="138" t="s">
+        <v>524</v>
+      </c>
+      <c r="C85" s="113" t="s">
+        <v>290</v>
+      </c>
+      <c r="D85" s="114">
+        <v>0.94097222222222221</v>
+      </c>
+      <c r="E85" s="114">
+        <v>0.99305555555555547</v>
+      </c>
+      <c r="F85" s="114">
+        <f>E85-D85</f>
+        <v>5.2083333333333259E-2</v>
+      </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="132"/>
-      <c r="B86" s="107"/>
-      <c r="C86" s="129"/>
-      <c r="D86" s="130"/>
-      <c r="E86" s="130"/>
-      <c r="F86" s="130">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
+      <c r="B86" s="139"/>
+      <c r="C86" s="113"/>
+      <c r="D86" s="114"/>
+      <c r="E86" s="114"/>
+      <c r="F86" s="114"/>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="132"/>
       <c r="B87" s="107"/>
-      <c r="C87" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D87" s="108">
+      <c r="C87" s="129" t="s">
+        <v>290</v>
+      </c>
+      <c r="D87" s="130">
         <v>0.35416666666666669</v>
       </c>
-      <c r="E87" s="108">
+      <c r="E87" s="130">
         <v>0.36458333333333331</v>
       </c>
-      <c r="F87" s="108">
+      <c r="F87" s="130">
         <f t="shared" si="14"/>
         <v>1.041666666666663E-2</v>
       </c>
@@ -30706,7 +30741,7 @@
     <row r="122" spans="1:9">
       <c r="A122" s="136"/>
       <c r="B122" s="107" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>290</v>
@@ -30856,7 +30891,7 @@
     <row r="128" spans="1:9">
       <c r="A128" s="136"/>
       <c r="B128" s="107" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C128" s="107" t="s">
         <v>297</v>
@@ -30876,7 +30911,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="136"/>
       <c r="B129" s="107" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C129" s="111" t="s">
         <v>302</v>
@@ -31079,7 +31114,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C79:C84 C2:C77 C86:C139" xr:uid="{E11A071F-B02F-4004-8781-5995222CFFE1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C77 C79:C139" xr:uid="{E11A071F-B02F-4004-8781-5995222CFFE1}">
       <formula1>$Q$1:$Q$7</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
time sheet commited by kishore
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B2714CC-9079-404B-934D-9EE328C1347E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{94952CE5-C299-4CE0-9CF5-850454A640F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="24" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3174" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3176" uniqueCount="535">
   <si>
     <t>Resource Name</t>
   </si>
@@ -1973,6 +1973,18 @@
     <t xml:space="preserve">Explored on pagination in angular and integration of web api and angular </t>
   </si>
   <si>
+    <t>Worked on angular Profile Histroy Page</t>
+  </si>
+  <si>
+    <t>Worked on angular HR home page</t>
+  </si>
+  <si>
+    <t>Explored on Data Binding</t>
+  </si>
+  <si>
+    <t>Worked on angular Admin home page</t>
+  </si>
+  <si>
     <t>Timesheet filling</t>
   </si>
   <si>
@@ -1997,7 +2009,7 @@
     <t>Worked on angular and web api integration</t>
   </si>
   <si>
-    <t>Explored on Data Binding</t>
+    <t>College project review</t>
   </si>
   <si>
     <t>Customer Meeting and Discussion</t>
@@ -22388,7 +22400,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FEFA632-027C-44B7-B2E8-75A517756B1E}">
   <dimension ref="A1:Q142"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A99" workbookViewId="0">
       <selection activeCell="I137" sqref="I137"/>
     </sheetView>
   </sheetViews>
@@ -25245,8 +25257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9EFCF2-B647-4263-9741-7AEEC9FEC381}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28180,8 +28192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448AE304-61C3-4727-BB61-AC5EFF7EF149}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="B141" sqref="B141"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -29437,20 +29449,20 @@
         <v>62</v>
       </c>
       <c r="B58" s="107" t="s">
-        <v>466</v>
+        <v>521</v>
       </c>
       <c r="C58" s="107" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D58" s="108">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="E58" s="108">
         <v>0.4375</v>
       </c>
       <c r="F58" s="108">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>8.3333333333333315E-2</v>
       </c>
       <c r="H58" s="106" t="s">
         <v>291</v>
@@ -29462,7 +29474,7 @@
     <row r="59" spans="1:9">
       <c r="A59" s="134"/>
       <c r="B59" s="107" t="s">
-        <v>500</v>
+        <v>522</v>
       </c>
       <c r="C59" s="107" t="s">
         <v>290</v>
@@ -29471,18 +29483,18 @@
         <v>0.4375</v>
       </c>
       <c r="E59" s="108">
-        <v>0.45833333333333331</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="F59" s="108">
         <f t="shared" si="0"/>
-        <v>2.0833333333333315E-2</v>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="H59" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I59" s="108">
         <f t="shared" ref="I59" si="9">SUMIFS(F58:F73, C58:C73,H59)</f>
-        <v>0.12847222222222215</v>
+        <v>0.23263888888888895</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -29494,30 +29506,30 @@
         <v>299</v>
       </c>
       <c r="D60" s="108">
-        <v>0.45833333333333331</v>
+        <v>0.47222222222222227</v>
       </c>
       <c r="E60" s="108">
         <v>0.47916666666666669</v>
       </c>
       <c r="F60" s="108">
         <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="H60" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I60" s="108">
         <f t="shared" ref="I60" si="10">SUMIFS(F58:F73, C58:C73,H60)</f>
-        <v>5.5555555555555525E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="134"/>
       <c r="B61" s="107" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
       <c r="C61" s="107" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D61" s="108">
         <v>0.47916666666666669</v>
@@ -29534,7 +29546,7 @@
       </c>
       <c r="I61" s="108">
         <f t="shared" ref="I61" si="11">SUMIFS(F58:F73, C58:C73,H61)</f>
-        <v>0.10416666666666674</v>
+        <v>0.1736111111111111</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -29560,7 +29572,7 @@
       </c>
       <c r="I62" s="108">
         <f t="shared" ref="I62" si="12">SUMIFS(F58:F73, C58:C73,H62)</f>
-        <v>4.166666666666663E-2</v>
+        <v>1.736111111111116E-2</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -29612,52 +29624,52 @@
       </c>
       <c r="I64" s="108">
         <f>SUMIFS(F57:F72, C57:C72,H64)</f>
-        <v>6.9444444444444531E-2</v>
+        <v>5.5555555555555469E-2</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="134"/>
       <c r="B65" s="107" t="s">
-        <v>314</v>
+        <v>368</v>
       </c>
       <c r="C65" s="107" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D65" s="108">
-        <v>0.625</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E65" s="108">
-        <v>0.66666666666666663</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="F65" s="108">
         <f t="shared" si="0"/>
-        <v>4.166666666666663E-2</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="H65" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I65" s="106">
         <f>SUM(I58:I64)</f>
-        <v>0.46180555555555558</v>
+        <v>0.54166666666666674</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="134"/>
       <c r="B66" s="107" t="s">
-        <v>368</v>
+        <v>314</v>
       </c>
       <c r="C66" s="107" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="D66" s="108">
-        <v>0.66666666666666663</v>
+        <v>0.73263888888888884</v>
       </c>
       <c r="E66" s="108">
-        <v>0.6875</v>
+        <v>0.75</v>
       </c>
       <c r="F66" s="108">
         <f t="shared" si="0"/>
-        <v>2.083333333333337E-2</v>
+        <v>1.736111111111116E-2</v>
       </c>
       <c r="H66" s="105"/>
       <c r="I66" s="106"/>
@@ -29665,16 +29677,16 @@
     <row r="67" spans="1:9">
       <c r="A67" s="134"/>
       <c r="B67" s="107" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="C67" s="107" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="D67" s="108">
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="E67" s="108">
-        <v>0.74305555555555547</v>
+        <v>0.82638888888888884</v>
       </c>
       <c r="F67" s="108">
         <f t="shared" ref="F67:F130" si="14">E67-D67</f>
@@ -29685,7 +29697,7 @@
     <row r="68" spans="1:9">
       <c r="A68" s="134"/>
       <c r="B68" s="107" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
       <c r="C68" s="107" t="s">
         <v>290</v>
@@ -29694,23 +29706,31 @@
         <v>0.71875</v>
       </c>
       <c r="E68" s="108">
-        <v>0.75</v>
+        <v>0.74305555555555547</v>
       </c>
       <c r="F68" s="108">
         <f t="shared" si="14"/>
-        <v>3.125E-2</v>
+        <v>2.4305555555555469E-2</v>
       </c>
       <c r="I68" s="110"/>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="134"/>
-      <c r="B69" s="107"/>
-      <c r="C69" s="107"/>
-      <c r="D69" s="108"/>
-      <c r="E69" s="108"/>
+      <c r="B69" s="107" t="s">
+        <v>524</v>
+      </c>
+      <c r="C69" s="107" t="s">
+        <v>290</v>
+      </c>
+      <c r="D69" s="108">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="E69" s="108">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F69" s="108">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>9.0277777777777901E-2</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -29762,7 +29782,7 @@
         <v>67</v>
       </c>
       <c r="B74" s="107" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="C74" s="107" t="s">
         <v>295</v>
@@ -29787,7 +29807,7 @@
     <row r="75" spans="1:9">
       <c r="A75" s="134"/>
       <c r="B75" s="107" t="s">
-        <v>522</v>
+        <v>526</v>
       </c>
       <c r="C75" s="107" t="s">
         <v>290</v>
@@ -29813,7 +29833,7 @@
     <row r="76" spans="1:9">
       <c r="A76" s="134"/>
       <c r="B76" s="107" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="C76" s="107" t="s">
         <v>290</v>
@@ -29989,7 +30009,7 @@
     <row r="83" spans="1:9">
       <c r="A83" s="139"/>
       <c r="B83" s="113" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="C83" s="115" t="s">
         <v>290</v>
@@ -30009,7 +30029,7 @@
     <row r="84" spans="1:9">
       <c r="A84" s="139"/>
       <c r="B84" s="113" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="C84" s="116" t="s">
         <v>297</v>
@@ -30028,7 +30048,7 @@
     <row r="85" spans="1:9">
       <c r="A85" s="139"/>
       <c r="B85" s="132" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
       <c r="C85" s="113" t="s">
         <v>290</v>
@@ -30667,7 +30687,7 @@
         <v>339</v>
       </c>
       <c r="B119" s="115" t="s">
-        <v>526</v>
+        <v>530</v>
       </c>
       <c r="C119" s="107" t="s">
         <v>290</v>
@@ -30692,7 +30712,7 @@
     <row r="120" spans="1:9">
       <c r="A120" s="138"/>
       <c r="B120" s="115" t="s">
-        <v>527</v>
+        <v>531</v>
       </c>
       <c r="C120" s="107" t="s">
         <v>290</v>
@@ -30744,7 +30764,7 @@
     <row r="122" spans="1:9">
       <c r="A122" s="138"/>
       <c r="B122" s="107" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C122" s="107" t="s">
         <v>290</v>
@@ -30822,7 +30842,7 @@
     <row r="125" spans="1:9">
       <c r="A125" s="138"/>
       <c r="B125" s="107" t="s">
-        <v>296</v>
+        <v>533</v>
       </c>
       <c r="C125" s="107" t="s">
         <v>300</v>
@@ -30894,7 +30914,7 @@
     <row r="128" spans="1:9">
       <c r="A128" s="138"/>
       <c r="B128" s="107" t="s">
-        <v>528</v>
+        <v>532</v>
       </c>
       <c r="C128" s="107" t="s">
         <v>290</v>
@@ -30914,7 +30934,7 @@
     <row r="129" spans="1:9">
       <c r="A129" s="138"/>
       <c r="B129" s="107" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="C129" s="107" t="s">
         <v>297</v>
@@ -30933,7 +30953,7 @@
     <row r="130" spans="1:9">
       <c r="A130" s="138"/>
       <c r="B130" s="107" t="s">
-        <v>530</v>
+        <v>534</v>
       </c>
       <c r="C130" s="111" t="s">
         <v>302</v>

</xml_diff>

<commit_message>
Updated timesheet - chitrarasu
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA6852C9-A603-49C3-B7DF-3EB53D86BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8876B899-AD77-45AA-8699-369F8345F01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="33" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="30" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05-04-2022" sheetId="1" r:id="rId1"/>
@@ -8116,7 +8116,7 @@
     <col min="7" max="7" width="19.42578125" style="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -8399,7 +8399,7 @@
     <col min="8" max="8" width="29.140625" style="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="27.75">
+    <row r="2" spans="2:8" ht="30">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -8679,7 +8679,7 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="27.75">
+    <row r="2" spans="2:8" ht="30.75">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -8840,7 +8840,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="135">
+    <row r="9" spans="2:8" ht="148.5">
       <c r="B9" s="55" t="s">
         <v>28</v>
       </c>
@@ -8934,7 +8934,7 @@
     <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75">
+    <row r="1" spans="1:7" ht="45">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9188,7 +9188,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="45">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9442,7 +9442,7 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:8" ht="45">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -9603,7 +9603,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" ht="30">
       <c r="B9" s="55" t="s">
         <v>28</v>
       </c>
@@ -9626,7 +9626,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="38.25">
       <c r="B10" s="55" t="s">
         <v>19</v>
       </c>
@@ -9689,12 +9689,12 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="45">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9855,7 +9855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="74.25">
+    <row r="8" spans="1:7" ht="89.25">
       <c r="A8" s="55" t="s">
         <v>28</v>
       </c>
@@ -9878,7 +9878,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="38.25">
       <c r="A9" s="55" t="s">
         <v>19</v>
       </c>
@@ -10063,7 +10063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="183.75">
+    <row r="6" spans="1:7" ht="202.5">
       <c r="A6" s="59" t="s">
         <v>62</v>
       </c>
@@ -35928,8 +35928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854A00F8-992E-4B44-9F90-36D78D50D69F}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38398,8 +38398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8ADE1-93B9-4EDE-A55C-8B6B4501AC81}">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41010,8 +41010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0830CE31-C1B7-48B7-899C-518D7217CA1B}">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43706,7 +43706,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="4:10" ht="27.75">
+    <row r="9" spans="4:10" ht="60.75">
       <c r="D9" s="20" t="s">
         <v>0</v>
       </c>
@@ -43964,8 +43964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9976145-3ED4-43FB-AC21-DC2985003151}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -46595,8 +46595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EDA147-041A-4AC2-943B-2A8852DD9324}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49170,8 +49170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2FCC25-CE88-4974-A988-E4673FD54BAF}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -51649,8 +51649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BA9E07-C648-4E9A-B718-CECE904D4C1C}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54072,8 +54072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE7F45E-1A36-42CF-A957-DFED1E93AECB}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56816,7 +56816,7 @@
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="27.75">
+    <row r="3" spans="1:7" ht="60.75">
       <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
@@ -57085,7 +57085,7 @@
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="54.75">
+    <row r="2" spans="1:7" ht="60.75">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -57269,7 +57269,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="25.5">
+    <row r="10" spans="1:7" ht="27">
       <c r="A10" s="39" t="s">
         <v>28</v>
       </c>
@@ -57360,7 +57360,7 @@
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75">
+    <row r="1" spans="1:7" ht="60.75">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -57406,7 +57406,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="61.5">
+    <row r="3" spans="1:7" ht="67.5">
       <c r="A3" s="55" t="s">
         <v>48</v>
       </c>
@@ -57452,7 +57452,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="61.5">
+    <row r="5" spans="1:7" ht="67.5">
       <c r="A5" s="55" t="s">
         <v>54</v>
       </c>
@@ -57498,7 +57498,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="108">
+    <row r="7" spans="1:7" ht="121.5">
       <c r="A7" s="59" t="s">
         <v>62</v>
       </c>
@@ -57631,7 +57631,7 @@
     <col min="3" max="3" width="55" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -57912,7 +57912,7 @@
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.75">
+    <row r="1" spans="1:7" ht="30">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -57981,7 +57981,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="30.75">
       <c r="A4" s="55" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
commit yoga service and timesheet
</commit_message>
<xml_diff>
--- a/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
+++ b/Process/Timesheet/PTW-TimeSheet 2 (1).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25311"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8876B899-AD77-45AA-8699-369F8345F01E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{91095F60-9798-4BBA-BA4A-53327A9316AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="30" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="33" activeTab="33" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="05-04-2022" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5273" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5231" uniqueCount="750">
   <si>
     <t>Resource Name</t>
   </si>
@@ -2502,6 +2502,9 @@
     <t>Worked on services for user and profile in angular</t>
   </si>
   <si>
+    <t>Worked on profile details angular and routing</t>
+  </si>
+  <si>
     <t>Modified Profile service(Profile)</t>
   </si>
   <si>
@@ -2556,6 +2559,15 @@
     <t>Created Models for Profile History Serices</t>
   </si>
   <si>
+    <t>Worked on profile service (profile)</t>
+  </si>
+  <si>
+    <t>Worked on API integration for profile service</t>
+  </si>
+  <si>
+    <t>Tested profile service in swagger</t>
+  </si>
+  <si>
     <t>college work</t>
   </si>
   <si>
@@ -2596,6 +2608,9 @@
   </si>
   <si>
     <t>Worked on personal service API</t>
+  </si>
+  <si>
+    <t>Absent(Vacated PG and Travelled to native)</t>
   </si>
   <si>
     <t>Modified profile service(Profile model)</t>
@@ -8116,7 +8131,7 @@
     <col min="7" max="7" width="19.42578125" style="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -8399,7 +8414,7 @@
     <col min="8" max="8" width="29.140625" style="79" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="30">
+    <row r="2" spans="2:8" ht="27.75">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -8679,7 +8694,7 @@
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="30.75">
+    <row r="2" spans="2:8" ht="27.75">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -8840,7 +8855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="148.5">
+    <row r="9" spans="2:8" ht="135">
       <c r="B9" s="55" t="s">
         <v>28</v>
       </c>
@@ -8934,7 +8949,7 @@
     <col min="7" max="7" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9188,7 +9203,7 @@
     <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9442,7 +9457,7 @@
     <col min="8" max="8" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="45">
+    <row r="2" spans="2:8">
       <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
@@ -9603,7 +9618,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="30">
+    <row r="9" spans="2:8">
       <c r="B9" s="55" t="s">
         <v>28</v>
       </c>
@@ -9626,7 +9641,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="38.25">
+    <row r="10" spans="2:8">
       <c r="B10" s="55" t="s">
         <v>19</v>
       </c>
@@ -9689,12 +9704,12 @@
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="43.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
     <col min="6" max="6" width="26.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45">
+    <row r="1" spans="1:7">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -9855,7 +9870,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="89.25">
+    <row r="8" spans="1:7" ht="74.25">
       <c r="A8" s="55" t="s">
         <v>28</v>
       </c>
@@ -9878,7 +9893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="55" t="s">
         <v>19</v>
       </c>
@@ -10063,7 +10078,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="202.5">
+    <row r="6" spans="1:7" ht="183.75">
       <c r="A6" s="59" t="s">
         <v>62</v>
       </c>
@@ -35928,8 +35943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854A00F8-992E-4B44-9F90-36D78D50D69F}">
   <dimension ref="A1:Q141"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -38398,8 +38413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2B8ADE1-93B9-4EDE-A55C-8B6B4501AC81}">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -41010,8 +41025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0830CE31-C1B7-48B7-899C-518D7217CA1B}">
   <dimension ref="A1:Q126"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -43706,7 +43721,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="4:10" ht="60.75">
+    <row r="9" spans="4:10" ht="27.75">
       <c r="D9" s="20" t="s">
         <v>0</v>
       </c>
@@ -43964,8 +43979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9976145-3ED4-43FB-AC21-DC2985003151}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -46181,7 +46196,7 @@
         <v>339</v>
       </c>
       <c r="B107" s="115" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="C107" s="113" t="s">
         <v>290</v>
@@ -46595,8 +46610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EDA147-041A-4AC2-943B-2A8852DD9324}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -48756,7 +48771,7 @@
         <v>339</v>
       </c>
       <c r="B107" s="115" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="C107" s="113" t="s">
         <v>290</v>
@@ -48786,22 +48801,22 @@
       <c r="C108" s="113" t="s">
         <v>290</v>
       </c>
-      <c r="D108" s="114">
-        <v>0.42708333333333331</v>
+      <c r="D108" s="108">
+        <v>0.38541666666666669</v>
       </c>
       <c r="E108" s="114">
-        <v>0.47222222222222227</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="F108" s="114">
         <f>E108-D108</f>
-        <v>4.5138888888888951E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="H108" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I108" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H108)</f>
-        <v>0.25694444444444442</v>
+        <v>0.25694444444444431</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -48813,14 +48828,14 @@
         <v>299</v>
       </c>
       <c r="D109" s="114">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="E109" s="114">
         <v>0.47222222222222227</v>
-      </c>
-      <c r="E109" s="114">
-        <v>0.47916666666666669</v>
       </c>
       <c r="F109" s="114">
         <f>E109-D109</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.3888888888888951E-2</v>
       </c>
       <c r="H109" s="109" t="s">
         <v>295</v>
@@ -48853,7 +48868,7 @@
       </c>
       <c r="I110" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H110)</f>
-        <v>5.208333333333337E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:9">
@@ -48879,7 +48894,7 @@
       </c>
       <c r="I111" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H111)</f>
-        <v>1.388888888888884E-2</v>
+        <v>2.777777777777779E-2</v>
       </c>
     </row>
     <row r="112" spans="1:9">
@@ -48894,11 +48909,11 @@
         <v>0.54861111111111105</v>
       </c>
       <c r="E112" s="114">
-        <v>0.57291666666666663</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="F112" s="114">
         <f>E112-D112</f>
-        <v>2.430555555555558E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H112" s="109" t="s">
         <v>302</v>
@@ -48911,72 +48926,72 @@
     <row r="113" spans="1:9">
       <c r="A113" s="153"/>
       <c r="B113" s="113" t="s">
-        <v>671</v>
+        <v>694</v>
       </c>
       <c r="C113" s="113" t="s">
         <v>290</v>
       </c>
       <c r="D113" s="114">
-        <v>0.57291666666666663</v>
+        <v>0.56944444444444442</v>
       </c>
       <c r="E113" s="114">
-        <v>0.65972222222222221</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="F113" s="114">
         <f>E113-D113</f>
-        <v>8.680555555555558E-2</v>
+        <v>7.6388888888888951E-2</v>
       </c>
       <c r="H113" s="109" t="s">
         <v>299</v>
       </c>
       <c r="I113" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H113)</f>
-        <v>4.861111111111116E-2</v>
+        <v>5.2083333333333481E-2</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="153"/>
       <c r="B114" s="113" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="C114" s="113" t="s">
-        <v>299</v>
-      </c>
-      <c r="D114" s="114">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="E114" s="114">
-        <v>0.67708333333333337</v>
+        <v>300</v>
+      </c>
+      <c r="D114" s="108">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E114" s="108">
+        <v>0.67361111111111116</v>
       </c>
       <c r="F114" s="114">
         <f>E114-D114</f>
-        <v>1.736111111111116E-2</v>
+        <v>2.777777777777779E-2</v>
       </c>
       <c r="H114" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I114" s="106">
         <f>SUM(I108:I113)</f>
-        <v>0.41319444444444448</v>
+        <v>0.37847222222222227</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="153"/>
       <c r="B115" s="113" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C115" s="113" t="s">
-        <v>300</v>
-      </c>
-      <c r="D115" s="114">
+        <v>299</v>
+      </c>
+      <c r="D115" s="108">
         <v>0.67708333333333337</v>
       </c>
-      <c r="E115" s="114">
-        <v>0.69097222222222221</v>
+      <c r="E115" s="108">
+        <v>0.69444444444444453</v>
       </c>
       <c r="F115" s="114">
         <f>E115-D115</f>
-        <v>1.388888888888884E-2</v>
+        <v>1.736111111111116E-2</v>
       </c>
       <c r="I115" s="110"/>
     </row>
@@ -48989,54 +49004,32 @@
         <v>290</v>
       </c>
       <c r="D116" s="114">
-        <v>0.69097222222222221</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="E116" s="114">
         <v>0.76041666666666663</v>
       </c>
       <c r="F116" s="114">
         <f>E116-D116</f>
-        <v>6.944444444444442E-2</v>
+        <v>6.5972222222222099E-2</v>
       </c>
       <c r="I116" s="110"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="153"/>
-      <c r="B117" s="142" t="s">
-        <v>673</v>
-      </c>
-      <c r="C117" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D117" s="114">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="E117" s="114">
-        <v>0.77430555555555547</v>
-      </c>
-      <c r="F117" s="114">
-        <f>E117-D117</f>
-        <v>1.388888888888884E-2</v>
-      </c>
+      <c r="B117" s="142"/>
+      <c r="C117" s="113"/>
+      <c r="D117" s="114"/>
+      <c r="E117" s="114"/>
+      <c r="F117" s="114"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="153"/>
-      <c r="B118" s="113" t="s">
-        <v>674</v>
-      </c>
-      <c r="C118" s="113" t="s">
-        <v>297</v>
-      </c>
-      <c r="D118" s="114">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="E118" s="114">
-        <v>0.90625</v>
-      </c>
-      <c r="F118" s="114">
-        <f>E118-D118</f>
-        <v>5.208333333333337E-2</v>
-      </c>
+      <c r="B118" s="113"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="114"/>
+      <c r="E118" s="114"/>
+      <c r="F118" s="114"/>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="153"/>
@@ -49170,8 +49163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2FCC25-CE88-4974-A988-E4673FD54BAF}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="M120" sqref="M120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49217,7 +49210,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="107" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="C2" s="107" t="s">
         <v>290</v>
@@ -49332,7 +49325,7 @@
     <row r="6" spans="1:17">
       <c r="A6" s="157"/>
       <c r="B6" s="107" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>290</v>
@@ -49390,7 +49383,7 @@
     <row r="8" spans="1:17">
       <c r="A8" s="157"/>
       <c r="B8" s="107" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="C8" s="107" t="s">
         <v>290</v>
@@ -49416,7 +49409,7 @@
     <row r="9" spans="1:17">
       <c r="A9" s="157"/>
       <c r="B9" s="107" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C9" s="107" t="s">
         <v>295</v>
@@ -49548,7 +49541,7 @@
     <row r="18" spans="1:9">
       <c r="A18" s="149"/>
       <c r="B18" s="107" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="C18" s="107" t="s">
         <v>290</v>
@@ -49600,7 +49593,7 @@
     <row r="20" spans="1:9">
       <c r="A20" s="149"/>
       <c r="B20" s="107" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C20" s="107" t="s">
         <v>290</v>
@@ -49652,7 +49645,7 @@
     <row r="22" spans="1:9">
       <c r="A22" s="149"/>
       <c r="B22" s="107" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>295</v>
@@ -49678,7 +49671,7 @@
     <row r="23" spans="1:9">
       <c r="A23" s="149"/>
       <c r="B23" s="107" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="C23" s="107" t="s">
         <v>290</v>
@@ -50124,7 +50117,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="149"/>
       <c r="B48" s="107" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>290</v>
@@ -50176,7 +50169,7 @@
     <row r="50" spans="1:9">
       <c r="A50" s="149"/>
       <c r="B50" s="107" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="C50" s="107" t="s">
         <v>290</v>
@@ -50228,7 +50221,7 @@
     <row r="52" spans="1:9">
       <c r="A52" s="149"/>
       <c r="B52" s="107" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="C52" s="107" t="s">
         <v>295</v>
@@ -50371,7 +50364,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="107" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C62" s="107" t="s">
         <v>290</v>
@@ -50422,7 +50415,7 @@
     <row r="64" spans="1:9">
       <c r="A64" s="149"/>
       <c r="B64" s="107" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C64" s="107" t="s">
         <v>295</v>
@@ -50474,7 +50467,7 @@
     <row r="66" spans="1:9">
       <c r="A66" s="149"/>
       <c r="B66" s="107" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="C66" s="107" t="s">
         <v>290</v>
@@ -50500,7 +50493,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="149"/>
       <c r="B67" s="107" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>290</v>
@@ -50552,7 +50545,7 @@
     <row r="69" spans="1:9">
       <c r="A69" s="149"/>
       <c r="B69" s="120" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C69" s="107" t="s">
         <v>290</v>
@@ -50659,15 +50652,9 @@
         <v>67</v>
       </c>
       <c r="B77" s="115"/>
-      <c r="C77" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D77" s="108">
-        <v>0</v>
-      </c>
-      <c r="E77" s="108">
-        <v>0</v>
-      </c>
+      <c r="C77" s="107"/>
+      <c r="D77" s="108"/>
+      <c r="E77" s="108"/>
       <c r="F77" s="108">
         <f>E77-D77</f>
         <v>0</v>
@@ -50682,17 +50669,11 @@
     <row r="78" spans="1:9">
       <c r="A78" s="153"/>
       <c r="B78" s="115" t="s">
-        <v>708</v>
-      </c>
-      <c r="C78" s="107" t="s">
-        <v>295</v>
-      </c>
-      <c r="D78" s="108">
-        <v>0</v>
-      </c>
-      <c r="E78" s="108">
-        <v>0</v>
-      </c>
+        <v>709</v>
+      </c>
+      <c r="C78" s="107"/>
+      <c r="D78" s="108"/>
+      <c r="E78" s="108"/>
       <c r="F78" s="108">
         <f>E78-D78</f>
         <v>0</v>
@@ -50708,15 +50689,9 @@
     <row r="79" spans="1:9">
       <c r="A79" s="153"/>
       <c r="B79" s="115"/>
-      <c r="C79" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D79" s="108">
-        <v>0</v>
-      </c>
-      <c r="E79" s="108">
-        <v>0</v>
-      </c>
+      <c r="C79" s="107"/>
+      <c r="D79" s="108"/>
+      <c r="E79" s="108"/>
       <c r="F79" s="108">
         <f>E79-D79</f>
         <v>0</v>
@@ -50732,15 +50707,9 @@
     <row r="80" spans="1:9">
       <c r="A80" s="153"/>
       <c r="B80" s="115"/>
-      <c r="C80" s="107" t="s">
-        <v>295</v>
-      </c>
-      <c r="D80" s="108">
-        <v>0</v>
-      </c>
-      <c r="E80" s="108">
-        <v>0</v>
-      </c>
+      <c r="C80" s="107"/>
+      <c r="D80" s="108"/>
+      <c r="E80" s="108"/>
       <c r="F80" s="108">
         <f>E80-D80</f>
         <v>0</v>
@@ -50756,15 +50725,9 @@
     <row r="81" spans="1:9">
       <c r="A81" s="153"/>
       <c r="B81" s="115"/>
-      <c r="C81" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="D81" s="108">
-        <v>0</v>
-      </c>
-      <c r="E81" s="108">
-        <v>0</v>
-      </c>
+      <c r="C81" s="107"/>
+      <c r="D81" s="108"/>
+      <c r="E81" s="108"/>
       <c r="F81" s="108">
         <f>E81-D81</f>
         <v>0</v>
@@ -50780,15 +50743,9 @@
     <row r="82" spans="1:9">
       <c r="A82" s="153"/>
       <c r="B82" s="115"/>
-      <c r="C82" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="D82" s="108">
-        <v>0</v>
-      </c>
-      <c r="E82" s="108">
-        <v>0</v>
-      </c>
+      <c r="C82" s="107"/>
+      <c r="D82" s="108"/>
+      <c r="E82" s="108"/>
       <c r="F82" s="108">
         <f>E82-D82</f>
         <v>0</v>
@@ -50804,15 +50761,9 @@
     <row r="83" spans="1:9">
       <c r="A83" s="153"/>
       <c r="B83" s="115"/>
-      <c r="C83" s="107" t="s">
-        <v>299</v>
-      </c>
-      <c r="D83" s="108">
-        <v>0</v>
-      </c>
-      <c r="E83" s="108">
-        <v>0</v>
-      </c>
+      <c r="C83" s="107"/>
+      <c r="D83" s="108"/>
+      <c r="E83" s="108"/>
       <c r="F83" s="108">
         <f>E83-D83</f>
         <v>0</v>
@@ -50828,15 +50779,9 @@
     <row r="84" spans="1:9">
       <c r="A84" s="153"/>
       <c r="B84" s="115"/>
-      <c r="C84" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D84" s="108">
-        <v>0</v>
-      </c>
-      <c r="E84" s="108">
-        <v>0</v>
-      </c>
+      <c r="C84" s="107"/>
+      <c r="D84" s="108"/>
+      <c r="E84" s="108"/>
       <c r="F84" s="108">
         <f>E84-D84</f>
         <v>0</v>
@@ -50852,15 +50797,9 @@
     <row r="85" spans="1:9">
       <c r="A85" s="153"/>
       <c r="B85" s="115"/>
-      <c r="C85" s="107" t="s">
-        <v>290</v>
-      </c>
-      <c r="D85" s="108">
-        <v>0</v>
-      </c>
-      <c r="E85" s="108">
-        <v>0</v>
-      </c>
+      <c r="C85" s="107"/>
+      <c r="D85" s="108"/>
+      <c r="E85" s="108"/>
       <c r="F85" s="108">
         <f>E85-D85</f>
         <v>0</v>
@@ -50939,7 +50878,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="107" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C92" s="107" t="s">
         <v>290</v>
@@ -50990,7 +50929,7 @@
     <row r="94" spans="1:9">
       <c r="A94" s="149"/>
       <c r="B94" s="107" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="C94" s="107" t="s">
         <v>290</v>
@@ -51068,7 +51007,7 @@
     <row r="97" spans="1:9">
       <c r="A97" s="149"/>
       <c r="B97" s="107" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="C97" s="107" t="s">
         <v>290</v>
@@ -51235,20 +51174,20 @@
         <v>339</v>
       </c>
       <c r="B107" s="115" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="C107" s="113" t="s">
         <v>290</v>
       </c>
       <c r="D107" s="108">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="E107" s="108">
         <v>0.37152777777777773</v>
-      </c>
-      <c r="E107" s="108">
-        <v>0.38541666666666669</v>
       </c>
       <c r="F107" s="114">
         <f>E107-D107</f>
-        <v>1.3888888888888951E-2</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="H107" s="106" t="s">
         <v>291</v>
@@ -51260,27 +51199,27 @@
     <row r="108" spans="1:9">
       <c r="A108" s="153"/>
       <c r="B108" s="113" t="s">
-        <v>669</v>
+        <v>713</v>
       </c>
       <c r="C108" s="113" t="s">
         <v>290</v>
       </c>
-      <c r="D108" s="114">
-        <v>0.42708333333333331</v>
+      <c r="D108" s="108">
+        <v>0.37152777777777773</v>
       </c>
       <c r="E108" s="114">
-        <v>0.47222222222222227</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F108" s="114">
         <f>E108-D108</f>
-        <v>4.5138888888888951E-2</v>
+        <v>0.10763888888888895</v>
       </c>
       <c r="H108" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I108" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H108)</f>
-        <v>0.25694444444444442</v>
+        <v>0.2638888888888889</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -51292,92 +51231,92 @@
         <v>299</v>
       </c>
       <c r="D109" s="114">
-        <v>0.47222222222222227</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="E109" s="114">
-        <v>0.47916666666666669</v>
+        <v>0.49652777777777773</v>
       </c>
       <c r="F109" s="114">
         <f>E109-D109</f>
-        <v>6.9444444444444198E-3</v>
+        <v>1.7361111111111049E-2</v>
       </c>
       <c r="H109" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I109" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H109)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="153"/>
       <c r="B110" s="107" t="s">
-        <v>509</v>
+        <v>714</v>
       </c>
       <c r="C110" s="113" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D110" s="114">
-        <v>0.47916666666666669</v>
+        <v>0.49652777777777773</v>
       </c>
       <c r="E110" s="114">
-        <v>0.52083333333333337</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="F110" s="114">
         <f>E110-D110</f>
-        <v>4.1666666666666685E-2</v>
+        <v>5.9027777777777846E-2</v>
       </c>
       <c r="H110" s="109" t="s">
         <v>297</v>
       </c>
       <c r="I110" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H110)</f>
-        <v>5.208333333333337E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="153"/>
       <c r="B111" s="113" t="s">
-        <v>670</v>
+        <v>298</v>
       </c>
       <c r="C111" s="113" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D111" s="114">
-        <v>0.52083333333333337</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="E111" s="114">
-        <v>0.54861111111111105</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F111" s="114">
         <f>E111-D111</f>
-        <v>2.7777777777777679E-2</v>
+        <v>3.472222222222221E-2</v>
       </c>
       <c r="H111" s="109" t="s">
         <v>300</v>
       </c>
       <c r="I111" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H111)</f>
-        <v>1.388888888888884E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="153"/>
       <c r="B112" s="113" t="s">
-        <v>298</v>
+        <v>715</v>
       </c>
       <c r="C112" s="113" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="D112" s="114">
-        <v>0.54861111111111105</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="E112" s="114">
-        <v>0.57291666666666663</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="F112" s="114">
         <f>E112-D112</f>
-        <v>2.430555555555558E-2</v>
+        <v>9.0277777777777679E-2</v>
       </c>
       <c r="H112" s="109" t="s">
         <v>302</v>
@@ -51390,131 +51329,91 @@
     <row r="113" spans="1:9">
       <c r="A113" s="153"/>
       <c r="B113" s="113" t="s">
-        <v>671</v>
+        <v>303</v>
       </c>
       <c r="C113" s="113" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D113" s="114">
-        <v>0.57291666666666663</v>
+        <v>0.68055555555555547</v>
       </c>
       <c r="E113" s="114">
-        <v>0.65972222222222221</v>
+        <v>0.69444444444444453</v>
       </c>
       <c r="F113" s="114">
         <f>E113-D113</f>
-        <v>8.680555555555558E-2</v>
+        <v>1.3888888888889062E-2</v>
       </c>
       <c r="H113" s="109" t="s">
         <v>299</v>
       </c>
       <c r="I113" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H113)</f>
-        <v>4.861111111111116E-2</v>
+        <v>6.5972222222222321E-2</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="153"/>
-      <c r="B114" s="113" t="s">
-        <v>303</v>
-      </c>
-      <c r="C114" s="113" t="s">
-        <v>299</v>
-      </c>
-      <c r="D114" s="114">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="E114" s="114">
-        <v>0.67708333333333337</v>
-      </c>
+      <c r="B114" s="113"/>
+      <c r="C114" s="113"/>
+      <c r="D114" s="114"/>
+      <c r="E114" s="114"/>
       <c r="F114" s="114">
         <f>E114-D114</f>
-        <v>1.736111111111116E-2</v>
+        <v>0</v>
       </c>
       <c r="H114" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I114" s="106">
         <f>SUM(I108:I113)</f>
-        <v>0.41319444444444448</v>
+        <v>0.32986111111111122</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="153"/>
-      <c r="B115" s="113" t="s">
-        <v>296</v>
-      </c>
-      <c r="C115" s="113" t="s">
-        <v>300</v>
-      </c>
-      <c r="D115" s="114">
-        <v>0.67708333333333337</v>
-      </c>
-      <c r="E115" s="114">
-        <v>0.69097222222222221</v>
-      </c>
+      <c r="B115" s="113"/>
+      <c r="C115" s="113"/>
+      <c r="D115" s="114"/>
+      <c r="E115" s="114"/>
       <c r="F115" s="114">
         <f>E115-D115</f>
-        <v>1.388888888888884E-2</v>
+        <v>0</v>
       </c>
       <c r="I115" s="110"/>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="153"/>
-      <c r="B116" s="113" t="s">
-        <v>672</v>
-      </c>
-      <c r="C116" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D116" s="114">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="E116" s="114">
-        <v>0.76041666666666663</v>
-      </c>
+      <c r="B116" s="113"/>
+      <c r="C116" s="113"/>
+      <c r="D116" s="114"/>
+      <c r="E116" s="114"/>
       <c r="F116" s="114">
         <f>E116-D116</f>
-        <v>6.944444444444442E-2</v>
+        <v>0</v>
       </c>
       <c r="I116" s="110"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="153"/>
-      <c r="B117" s="142" t="s">
-        <v>673</v>
-      </c>
-      <c r="C117" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D117" s="114">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="E117" s="114">
-        <v>0.77430555555555547</v>
-      </c>
+      <c r="B117" s="142"/>
+      <c r="C117" s="113"/>
+      <c r="D117" s="114"/>
+      <c r="E117" s="114"/>
       <c r="F117" s="114">
         <f>E117-D117</f>
-        <v>1.388888888888884E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="153"/>
-      <c r="B118" s="113" t="s">
-        <v>674</v>
-      </c>
-      <c r="C118" s="113" t="s">
-        <v>297</v>
-      </c>
-      <c r="D118" s="114">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="E118" s="114">
-        <v>0.90625</v>
-      </c>
+      <c r="B118" s="113"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="114"/>
+      <c r="E118" s="114"/>
       <c r="F118" s="114">
         <f>E118-D118</f>
-        <v>5.208333333333337E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:9">
@@ -51649,8 +51548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BA9E07-C648-4E9A-B718-CECE904D4C1C}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -52003,7 +51902,7 @@
     <row r="18" spans="1:9">
       <c r="A18" s="149"/>
       <c r="B18" s="107" t="s">
-        <v>712</v>
+        <v>716</v>
       </c>
       <c r="C18" s="107" t="s">
         <v>295</v>
@@ -52107,7 +52006,7 @@
     <row r="22" spans="1:9">
       <c r="A22" s="149"/>
       <c r="B22" s="107" t="s">
-        <v>713</v>
+        <v>717</v>
       </c>
       <c r="C22" s="107" t="s">
         <v>290</v>
@@ -52159,7 +52058,7 @@
     <row r="24" spans="1:9">
       <c r="A24" s="149"/>
       <c r="B24" s="107" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="C24" s="107" t="s">
         <v>295</v>
@@ -52587,7 +52486,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="149"/>
       <c r="B48" s="107" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>295</v>
@@ -52665,7 +52564,7 @@
     <row r="51" spans="1:9">
       <c r="A51" s="149"/>
       <c r="B51" s="107" t="s">
-        <v>716</v>
+        <v>720</v>
       </c>
       <c r="C51" s="107" t="s">
         <v>290</v>
@@ -52717,7 +52616,7 @@
     <row r="53" spans="1:9">
       <c r="A53" s="149"/>
       <c r="B53" s="107" t="s">
-        <v>715</v>
+        <v>719</v>
       </c>
       <c r="C53" s="107" t="s">
         <v>295</v>
@@ -52867,7 +52766,7 @@
     <row r="63" spans="1:9">
       <c r="A63" s="149"/>
       <c r="B63" s="107" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="C63" s="107" t="s">
         <v>290</v>
@@ -52971,7 +52870,7 @@
     <row r="67" spans="1:9">
       <c r="A67" s="149"/>
       <c r="B67" s="107" t="s">
-        <v>718</v>
+        <v>722</v>
       </c>
       <c r="C67" s="107" t="s">
         <v>297</v>
@@ -53023,7 +52922,7 @@
     <row r="69" spans="1:9">
       <c r="A69" s="149"/>
       <c r="B69" s="107" t="s">
-        <v>719</v>
+        <v>723</v>
       </c>
       <c r="C69" s="107" t="s">
         <v>290</v>
@@ -53130,7 +53029,7 @@
         <v>67</v>
       </c>
       <c r="B77" s="115" t="s">
-        <v>720</v>
+        <v>724</v>
       </c>
       <c r="C77" s="107" t="s">
         <v>290</v>
@@ -53370,7 +53269,7 @@
         <v>28</v>
       </c>
       <c r="B92" s="107" t="s">
-        <v>721</v>
+        <v>725</v>
       </c>
       <c r="C92" s="107" t="s">
         <v>290</v>
@@ -53395,7 +53294,7 @@
     <row r="93" spans="1:9">
       <c r="A93" s="149"/>
       <c r="B93" s="107" t="s">
-        <v>722</v>
+        <v>726</v>
       </c>
       <c r="C93" s="107" t="s">
         <v>302</v>
@@ -53447,7 +53346,7 @@
     <row r="95" spans="1:9">
       <c r="A95" s="149"/>
       <c r="B95" s="107" t="s">
-        <v>723</v>
+        <v>727</v>
       </c>
       <c r="C95" s="107" t="s">
         <v>290</v>
@@ -53499,7 +53398,7 @@
     <row r="97" spans="1:9">
       <c r="A97" s="149"/>
       <c r="B97" s="107" t="s">
-        <v>724</v>
+        <v>728</v>
       </c>
       <c r="C97" s="107" t="s">
         <v>290</v>
@@ -53551,7 +53450,7 @@
     <row r="99" spans="1:9">
       <c r="A99" s="149"/>
       <c r="B99" s="138" t="s">
-        <v>725</v>
+        <v>729</v>
       </c>
       <c r="C99" s="138" t="s">
         <v>290</v>
@@ -53658,20 +53557,20 @@
         <v>339</v>
       </c>
       <c r="B107" s="115" t="s">
-        <v>557</v>
+        <v>539</v>
       </c>
       <c r="C107" s="113" t="s">
         <v>290</v>
       </c>
-      <c r="D107" s="108">
-        <v>0.37152777777777773</v>
+      <c r="D107" s="114">
+        <v>0.42708333333333331</v>
       </c>
       <c r="E107" s="108">
-        <v>0.38541666666666669</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="F107" s="114">
         <f>E107-D107</f>
-        <v>1.3888888888888951E-2</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="H107" s="106" t="s">
         <v>291</v>
@@ -53683,125 +53582,83 @@
     <row r="108" spans="1:9">
       <c r="A108" s="153"/>
       <c r="B108" s="113" t="s">
-        <v>669</v>
+        <v>294</v>
       </c>
       <c r="C108" s="113" t="s">
-        <v>290</v>
+        <v>300</v>
       </c>
       <c r="D108" s="114">
-        <v>0.42708333333333331</v>
+        <v>0.45833333333333331</v>
       </c>
       <c r="E108" s="114">
-        <v>0.47222222222222227</v>
+        <v>0.49305555555555558</v>
       </c>
       <c r="F108" s="114">
         <f>E108-D108</f>
-        <v>4.5138888888888951E-2</v>
+        <v>3.4722222222222265E-2</v>
       </c>
       <c r="H108" s="109" t="s">
         <v>290</v>
       </c>
       <c r="I108" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H108)</f>
-        <v>0.25694444444444442</v>
+        <v>6.9444444444444198E-3</v>
       </c>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="153"/>
       <c r="B109" s="113" t="s">
-        <v>301</v>
-      </c>
-      <c r="C109" s="113" t="s">
-        <v>299</v>
-      </c>
-      <c r="D109" s="114">
-        <v>0.47222222222222227</v>
-      </c>
-      <c r="E109" s="114">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="F109" s="114">
-        <f>E109-D109</f>
-        <v>6.9444444444444198E-3</v>
-      </c>
+        <v>730</v>
+      </c>
+      <c r="C109" s="113"/>
+      <c r="D109" s="114"/>
+      <c r="E109" s="114"/>
+      <c r="F109" s="114"/>
       <c r="H109" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I109" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H109)</f>
-        <v>4.1666666666666685E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" s="153"/>
-      <c r="B110" s="107" t="s">
-        <v>509</v>
-      </c>
-      <c r="C110" s="113" t="s">
-        <v>295</v>
-      </c>
-      <c r="D110" s="114">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="E110" s="114">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="F110" s="114">
-        <f>E110-D110</f>
-        <v>4.1666666666666685E-2</v>
-      </c>
+      <c r="B110" s="107"/>
+      <c r="C110" s="113"/>
+      <c r="D110" s="114"/>
+      <c r="E110" s="114"/>
+      <c r="F110" s="114"/>
       <c r="H110" s="109" t="s">
         <v>297</v>
       </c>
       <c r="I110" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H110)</f>
-        <v>5.208333333333337E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" s="153"/>
-      <c r="B111" s="113" t="s">
-        <v>670</v>
-      </c>
-      <c r="C111" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D111" s="114">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="E111" s="114">
-        <v>0.54861111111111105</v>
-      </c>
-      <c r="F111" s="114">
-        <f>E111-D111</f>
-        <v>2.7777777777777679E-2</v>
-      </c>
+      <c r="B111" s="113"/>
+      <c r="C111" s="113"/>
+      <c r="D111" s="114"/>
+      <c r="E111" s="114"/>
+      <c r="F111" s="114"/>
       <c r="H111" s="109" t="s">
         <v>300</v>
       </c>
       <c r="I111" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H111)</f>
-        <v>1.388888888888884E-2</v>
+        <v>3.4722222222222265E-2</v>
       </c>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" s="153"/>
-      <c r="B112" s="113" t="s">
-        <v>298</v>
-      </c>
-      <c r="C112" s="113" t="s">
-        <v>299</v>
-      </c>
-      <c r="D112" s="114">
-        <v>0.54861111111111105</v>
-      </c>
-      <c r="E112" s="114">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="F112" s="114">
-        <f>E112-D112</f>
-        <v>2.430555555555558E-2</v>
-      </c>
+      <c r="B112" s="113"/>
+      <c r="C112" s="113"/>
+      <c r="D112" s="114"/>
+      <c r="E112" s="114"/>
+      <c r="F112" s="114"/>
       <c r="H112" s="109" t="s">
         <v>302</v>
       </c>
@@ -53812,133 +53669,67 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113" s="153"/>
-      <c r="B113" s="113" t="s">
-        <v>671</v>
-      </c>
-      <c r="C113" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D113" s="114">
-        <v>0.57291666666666663</v>
-      </c>
-      <c r="E113" s="114">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="F113" s="114">
-        <f>E113-D113</f>
-        <v>8.680555555555558E-2</v>
-      </c>
+      <c r="B113" s="113"/>
+      <c r="C113" s="113"/>
+      <c r="D113" s="114"/>
+      <c r="E113" s="114"/>
+      <c r="F113" s="114"/>
       <c r="H113" s="109" t="s">
         <v>299</v>
       </c>
       <c r="I113" s="108">
         <f>SUMIFS(F107:F121, C107:C121,H113)</f>
-        <v>4.861111111111116E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" s="153"/>
-      <c r="B114" s="113" t="s">
-        <v>303</v>
-      </c>
-      <c r="C114" s="113" t="s">
-        <v>299</v>
-      </c>
-      <c r="D114" s="114">
-        <v>0.65972222222222221</v>
-      </c>
-      <c r="E114" s="114">
-        <v>0.67708333333333337</v>
-      </c>
-      <c r="F114" s="114">
-        <f>E114-D114</f>
-        <v>1.736111111111116E-2</v>
-      </c>
+      <c r="B114" s="113"/>
+      <c r="C114" s="113"/>
+      <c r="D114" s="114"/>
+      <c r="E114" s="114"/>
+      <c r="F114" s="114"/>
       <c r="H114" s="105" t="s">
         <v>305</v>
       </c>
       <c r="I114" s="106">
         <f>SUM(I108:I113)</f>
-        <v>0.41319444444444448</v>
+        <v>4.1666666666666685E-2</v>
       </c>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" s="153"/>
-      <c r="B115" s="113" t="s">
-        <v>296</v>
-      </c>
-      <c r="C115" s="113" t="s">
-        <v>300</v>
-      </c>
-      <c r="D115" s="114">
-        <v>0.67708333333333337</v>
-      </c>
-      <c r="E115" s="114">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="F115" s="114">
-        <f>E115-D115</f>
-        <v>1.388888888888884E-2</v>
-      </c>
+      <c r="B115" s="113"/>
+      <c r="C115" s="113"/>
+      <c r="D115" s="114"/>
+      <c r="E115" s="114"/>
+      <c r="F115" s="114"/>
       <c r="I115" s="110"/>
     </row>
     <row r="116" spans="1:9">
       <c r="A116" s="153"/>
-      <c r="B116" s="113" t="s">
-        <v>672</v>
-      </c>
-      <c r="C116" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D116" s="114">
-        <v>0.69097222222222221</v>
-      </c>
-      <c r="E116" s="114">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="F116" s="114">
-        <f>E116-D116</f>
-        <v>6.944444444444442E-2</v>
-      </c>
+      <c r="B116" s="113"/>
+      <c r="C116" s="113"/>
+      <c r="D116" s="114"/>
+      <c r="E116" s="114"/>
+      <c r="F116" s="114"/>
       <c r="I116" s="110"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="153"/>
-      <c r="B117" s="142" t="s">
-        <v>673</v>
-      </c>
-      <c r="C117" s="113" t="s">
-        <v>290</v>
-      </c>
-      <c r="D117" s="114">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="E117" s="114">
-        <v>0.77430555555555547</v>
-      </c>
-      <c r="F117" s="114">
-        <f>E117-D117</f>
-        <v>1.388888888888884E-2</v>
-      </c>
+      <c r="B117" s="142"/>
+      <c r="C117" s="113"/>
+      <c r="D117" s="114"/>
+      <c r="E117" s="114"/>
+      <c r="F117" s="114"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" s="153"/>
-      <c r="B118" s="113" t="s">
-        <v>674</v>
-      </c>
-      <c r="C118" s="113" t="s">
-        <v>297</v>
-      </c>
-      <c r="D118" s="114">
-        <v>0.85416666666666663</v>
-      </c>
-      <c r="E118" s="114">
-        <v>0.90625</v>
-      </c>
-      <c r="F118" s="114">
-        <f>E118-D118</f>
-        <v>5.208333333333337E-2</v>
-      </c>
+      <c r="B118" s="113"/>
+      <c r="C118" s="113"/>
+      <c r="D118" s="114"/>
+      <c r="E118" s="114"/>
+      <c r="F118" s="114"/>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="153"/>
@@ -54072,8 +53863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE7F45E-1A36-42CF-A957-DFED1E93AECB}">
   <dimension ref="A1:Q130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -54147,7 +53938,7 @@
     <row r="3" spans="1:17">
       <c r="A3" s="157"/>
       <c r="B3" s="107" t="s">
-        <v>726</v>
+        <v>731</v>
       </c>
       <c r="C3" s="107" t="s">
         <v>290</v>
@@ -54234,7 +54025,7 @@
     <row r="6" spans="1:17">
       <c r="A6" s="157"/>
       <c r="B6" s="107" t="s">
-        <v>727</v>
+        <v>732</v>
       </c>
       <c r="C6" s="107" t="s">
         <v>290</v>
@@ -54263,7 +54054,7 @@
     <row r="7" spans="1:17">
       <c r="A7" s="157"/>
       <c r="B7" s="107" t="s">
-        <v>728</v>
+        <v>733</v>
       </c>
       <c r="C7" s="107" t="s">
         <v>290</v>
@@ -54434,7 +54225,7 @@
     <row r="18" spans="1:9">
       <c r="A18" s="149"/>
       <c r="B18" s="107" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="C18" s="107" t="s">
         <v>295</v>
@@ -54486,7 +54277,7 @@
     <row r="20" spans="1:9">
       <c r="A20" s="149"/>
       <c r="B20" s="107" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="C20" s="107" t="s">
         <v>295</v>
@@ -54512,7 +54303,7 @@
     <row r="21" spans="1:9">
       <c r="A21" s="149"/>
       <c r="B21" s="107" t="s">
-        <v>731</v>
+        <v>736</v>
       </c>
       <c r="C21" s="107" t="s">
         <v>290</v>
@@ -55002,7 +54793,7 @@
     <row r="48" spans="1:9">
       <c r="A48" s="149"/>
       <c r="B48" s="107" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="C48" s="107" t="s">
         <v>295</v>
@@ -55028,7 +54819,7 @@
     <row r="49" spans="1:9">
       <c r="A49" s="149"/>
       <c r="B49" s="107" t="s">
-        <v>732</v>
+        <v>737</v>
       </c>
       <c r="C49" s="107" t="s">
         <v>290</v>
@@ -55106,7 +54897,7 @@
     <row r="52" spans="1:9">
       <c r="A52" s="149"/>
       <c r="B52" s="107" t="s">
-        <v>730</v>
+        <v>735</v>
       </c>
       <c r="C52" s="107" t="s">
         <v>295</v>
@@ -55326,7 +55117,7 @@
     <row r="65" spans="1:9">
       <c r="A65" s="149"/>
       <c r="B65" s="107" t="s">
-        <v>733</v>
+        <v>738</v>
       </c>
       <c r="C65" s="107" t="s">
         <v>299</v>
@@ -55352,7 +55143,7 @@
     <row r="66" spans="1:9">
       <c r="A66" s="149"/>
       <c r="B66" s="107" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="C66" s="107" t="s">
         <v>297</v>
@@ -55456,7 +55247,7 @@
     <row r="70" spans="1:9">
       <c r="A70" s="149"/>
       <c r="B70" s="107" t="s">
-        <v>735</v>
+        <v>740</v>
       </c>
       <c r="C70" s="107" t="s">
         <v>295</v>
@@ -55476,7 +55267,7 @@
     <row r="71" spans="1:9">
       <c r="A71" s="149"/>
       <c r="B71" s="107" t="s">
-        <v>736</v>
+        <v>741</v>
       </c>
       <c r="C71" s="107" t="s">
         <v>295</v>
@@ -55578,7 +55369,7 @@
     <row r="78" spans="1:9">
       <c r="A78" s="153"/>
       <c r="B78" s="115" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="C78" s="107" t="s">
         <v>295</v>
@@ -55630,7 +55421,7 @@
     <row r="80" spans="1:9">
       <c r="A80" s="153"/>
       <c r="B80" s="115" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="C80" s="107" t="s">
         <v>295</v>
@@ -55682,7 +55473,7 @@
     <row r="82" spans="1:9">
       <c r="A82" s="153"/>
       <c r="B82" s="115" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="C82" s="107" t="s">
         <v>290</v>
@@ -55708,7 +55499,7 @@
     <row r="83" spans="1:9">
       <c r="A83" s="153"/>
       <c r="B83" s="115" t="s">
-        <v>737</v>
+        <v>742</v>
       </c>
       <c r="C83" s="107" t="s">
         <v>295</v>
@@ -55866,7 +55657,7 @@
     <row r="93" spans="1:9">
       <c r="A93" s="149"/>
       <c r="B93" s="107" t="s">
-        <v>738</v>
+        <v>743</v>
       </c>
       <c r="C93" s="107" t="s">
         <v>295</v>
@@ -55892,7 +55683,7 @@
     <row r="94" spans="1:9">
       <c r="A94" s="149"/>
       <c r="B94" s="107" t="s">
-        <v>739</v>
+        <v>744</v>
       </c>
       <c r="C94" s="107" t="s">
         <v>290</v>
@@ -55918,7 +55709,7 @@
     <row r="95" spans="1:9">
       <c r="A95" s="149"/>
       <c r="B95" s="107" t="s">
-        <v>740</v>
+        <v>745</v>
       </c>
       <c r="C95" s="107" t="s">
         <v>295</v>
@@ -56130,7 +55921,7 @@
     <row r="108" spans="1:9">
       <c r="A108" s="153"/>
       <c r="B108" s="113" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="C108" s="113" t="s">
         <v>290</v>
@@ -56182,7 +55973,7 @@
     <row r="110" spans="1:9">
       <c r="A110" s="153"/>
       <c r="B110" s="113" t="s">
-        <v>741</v>
+        <v>746</v>
       </c>
       <c r="C110" s="113" t="s">
         <v>290</v>
@@ -56260,7 +56051,7 @@
     <row r="113" spans="1:9">
       <c r="A113" s="153"/>
       <c r="B113" s="113" t="s">
-        <v>742</v>
+        <v>747</v>
       </c>
       <c r="C113" s="113" t="s">
         <v>295</v>
@@ -56332,7 +56123,7 @@
     <row r="116" spans="1:9">
       <c r="A116" s="153"/>
       <c r="B116" s="113" t="s">
-        <v>743</v>
+        <v>748</v>
       </c>
       <c r="C116" s="113" t="s">
         <v>295</v>
@@ -56352,7 +56143,7 @@
     <row r="117" spans="1:9">
       <c r="A117" s="153"/>
       <c r="B117" s="142" t="s">
-        <v>744</v>
+        <v>749</v>
       </c>
       <c r="C117" s="113" t="s">
         <v>297</v>
@@ -56374,10 +56165,7 @@
       <c r="C118" s="113"/>
       <c r="D118" s="114"/>
       <c r="E118" s="114"/>
-      <c r="F118" s="114">
-        <f>E118-D118</f>
-        <v>0</v>
-      </c>
+      <c r="F118" s="114"/>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" s="153"/>
@@ -56816,7 +56604,7 @@
     <col min="7" max="7" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="60.75">
+    <row r="3" spans="1:7" ht="27.75">
       <c r="A3" s="31" t="s">
         <v>0</v>
       </c>
@@ -57085,7 +56873,7 @@
     <col min="3" max="3" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="60.75">
+    <row r="2" spans="1:7" ht="54.75">
       <c r="A2" s="31" t="s">
         <v>0</v>
       </c>
@@ -57269,7 +57057,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="27">
+    <row r="10" spans="1:7" ht="25.5">
       <c r="A10" s="39" t="s">
         <v>28</v>
       </c>
@@ -57360,7 +57148,7 @@
     <col min="7" max="7" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="60.75">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -57406,7 +57194,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="67.5">
+    <row r="3" spans="1:7" ht="61.5">
       <c r="A3" s="55" t="s">
         <v>48</v>
       </c>
@@ -57452,7 +57240,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="67.5">
+    <row r="5" spans="1:7" ht="61.5">
       <c r="A5" s="55" t="s">
         <v>54</v>
       </c>
@@ -57498,7 +57286,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="121.5">
+    <row r="7" spans="1:7" ht="108">
       <c r="A7" s="59" t="s">
         <v>62</v>
       </c>
@@ -57631,7 +57419,7 @@
     <col min="3" max="3" width="55" customWidth="1"/>
     <col min="4" max="4" width="23.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" customWidth="1"/>
     <col min="7" max="7" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -57912,7 +57700,7 @@
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30">
+    <row r="1" spans="1:7" ht="27.75">
       <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
@@ -57981,7 +57769,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30.75">
+    <row r="4" spans="1:7">
       <c r="A4" s="55" t="s">
         <v>41</v>
       </c>

</xml_diff>